<commit_message>
Add 0 in the Read offset
</commit_message>
<xml_diff>
--- a/atacseq/latest/atacseq.xlsx
+++ b/atacseq/latest/atacseq.xlsx
@@ -380,7 +380,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="370">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -802,12 +802,24 @@
     <t>https://identifiers.org/RRID:SCR_023694</t>
   </si>
   <si>
+    <t>NovaSeq X</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024569</t>
+  </si>
+  <si>
     <t>IN Cell Analyzer 2200</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_023616</t>
   </si>
   <si>
+    <t>NanoZoomer 2.0-HT</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_021658</t>
+  </si>
+  <si>
     <t>Lightsheet 7</t>
   </si>
   <si>
@@ -940,6 +952,18 @@
     <t>https://identifiers.org/RRID:SCR_023195</t>
   </si>
   <si>
+    <t>NovaSeq X Plus</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024568</t>
+  </si>
+  <si>
+    <t>NanoZoomer-SQ</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023763</t>
+  </si>
+  <si>
     <t>NextSeq 550</t>
   </si>
   <si>
@@ -1021,6 +1045,9 @@
     <t>barcode_offset</t>
   </si>
   <si>
+    <t>0</t>
+  </si>
+  <si>
     <t>Not applicable</t>
   </si>
   <si>
@@ -1033,6 +1060,12 @@
     <t>barcode_read</t>
   </si>
   <si>
+    <t>Read 1 (R1)</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C172301</t>
+  </si>
+  <si>
     <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C48660</t>
   </si>
   <si>
@@ -1066,12 +1099,6 @@
     <t>umi_read</t>
   </si>
   <si>
-    <t>Read 1 (R1)</t>
-  </si>
-  <si>
-    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C172301</t>
-  </si>
-  <si>
     <t>umi_size</t>
   </si>
   <si>
@@ -1195,18 +1222,18 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000250</t>
   </si>
   <si>
+    <t>Custom</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C126386</t>
+  </si>
+  <si>
     <t>10X Genomics; Visium Spatial Gene Expression Slide and Reagent Kit, 1 slides, 4 reactions; PN 1000187</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000265</t>
   </si>
   <si>
-    <t>Custom kit</t>
-  </si>
-  <si>
-    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C126386</t>
-  </si>
-  <si>
     <t>10X Genomics; Visium Spatial Gene Expression Slide and Reagent Kit, 4 slides, 16 reactions; PN 1000184</t>
   </si>
   <si>
@@ -1216,18 +1243,24 @@
     <t>sample_indexing_kit</t>
   </si>
   <si>
+    <t>10X Genomics; Dual Index Kit TS, Set A; PN 1000251</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000282</t>
+  </si>
+  <si>
+    <t>10X Genomics; Single Index Kit N, Set A (96 rxn); PN 1000212</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000252</t>
+  </si>
+  <si>
     <t>10X Genomics; Dual Index Kit TT, Set A (96 rxn); PN 1000215</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000253</t>
   </si>
   <si>
-    <t>10X Genomics; Single Index Kit N, Set A (96 rxn); PN 1000212</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000252</t>
-  </si>
-  <si>
     <t>sample_indexing_set</t>
   </si>
   <si>
@@ -1240,6 +1273,36 @@
     <t>sequencing_reagent_kit</t>
   </si>
   <si>
+    <t>Illumina; NovaSeq 6000 S4 Reagent v1.5 Kit (200 Cycles); PN 20028313</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000259</t>
+  </si>
+  <si>
+    <t>Illumina; NovaSeq X Series 1.5B Reagent Kit (100 Cycle); PN 20104703</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000286</t>
+  </si>
+  <si>
+    <t>Illumina; NovaSeq X Series 1.5B Reagent Kit (300 Cycle); PN 20104705</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000288</t>
+  </si>
+  <si>
+    <t>Illumina; NovaSeq 6000 S1 Reagent v1.5 Kit (100 Cycles); PN 20028319</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000257</t>
+  </si>
+  <si>
+    <t>Illumina; NovaSeq X Series 1.5B Reagent Kit (200 Cycle); PN 20104704</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000287</t>
+  </si>
+  <si>
     <t>Illumina; NovaSeq 6000 SP Reagent v1.5 Kit (100 Cycles); PN 20028401</t>
   </si>
   <si>
@@ -1252,16 +1315,22 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000254</t>
   </si>
   <si>
-    <t>Illumina; NovaSeq 6000 S4 Reagent v1.5 Kit (200 Cycles); PN 20028313</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000259</t>
-  </si>
-  <si>
-    <t>Illumina; NovaSeq 6000 S1 Reagent v1.5 Kit (100 Cycles); PN 20028319</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000257</t>
+    <t>Illumina; NovaSeq X Series 10B Reagent Kit (300 Cycle); PN 20085594</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000283</t>
+  </si>
+  <si>
+    <t>Illumina; NovaSeq X Series 10B Reagent Kit (200 Cycle); PN 20085595</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000284</t>
+  </si>
+  <si>
+    <t>Illumina; NovaSeq X Series 10B Reagent Kit (100 Cycle); PN 20085596</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000285</t>
   </si>
   <si>
     <t>Illumina; NovaSeq 6000 S2 Reagent v1.5 Kit (100 Cycles); PN 20028316</t>
@@ -1309,18 +1378,18 @@
     <t>preparation_instrument_vendor</t>
   </si>
   <si>
+    <t>HTX Technologies</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023734</t>
+  </si>
+  <si>
     <t>10x Genomics</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_023672</t>
   </si>
   <si>
-    <t>HTX Technologies</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023734</t>
-  </si>
-  <si>
     <t>SunChrom</t>
   </si>
   <si>
@@ -1330,16 +1399,34 @@
     <t>preparation_instrument_model</t>
   </si>
   <si>
+    <t>Sublimator</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023729</t>
+  </si>
+  <si>
+    <t>Chromium Controller</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_019326</t>
+  </si>
+  <si>
     <t>Chromium X</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_024537</t>
   </si>
   <si>
-    <t>Sublimator</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023729</t>
+    <t>AutoStainer XL</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023957</t>
+  </si>
+  <si>
+    <t>Visium CytAssist</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024570</t>
   </si>
   <si>
     <t>SunCollect Sprayer</t>
@@ -1354,12 +1441,6 @@
     <t>https://identifiers.org/RRID:SCR_023731</t>
   </si>
   <si>
-    <t>Chromium Controller</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_019326</t>
-  </si>
-  <si>
     <t>Chromium iX</t>
   </si>
   <si>
@@ -1402,7 +1483,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2023-10-06T19:20:18-07:00</t>
+    <t>2023-10-16T20:49:49-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1604,126 +1685,126 @@
         <v>131</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>220</v>
+        <v>231</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>226</v>
+        <v>237</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>227</v>
+        <v>238</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>230</v>
+        <v>239</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>234</v>
+        <v>243</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>245</v>
+        <v>254</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>246</v>
+        <v>255</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>248</v>
+        <v>257</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>249</v>
+        <v>258</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>253</v>
+        <v>262</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>254</v>
+        <v>263</v>
       </c>
       <c r="AD1" t="s" s="1">
-        <v>255</v>
+        <v>264</v>
       </c>
       <c r="AE1" t="s" s="1">
-        <v>258</v>
+        <v>267</v>
       </c>
       <c r="AF1" t="s" s="1">
-        <v>263</v>
+        <v>272</v>
       </c>
       <c r="AG1" t="s" s="1">
-        <v>264</v>
+        <v>273</v>
       </c>
       <c r="AH1" t="s" s="1">
-        <v>277</v>
+        <v>286</v>
       </c>
       <c r="AI1" t="s" s="1">
-        <v>282</v>
+        <v>293</v>
       </c>
       <c r="AJ1" t="s" s="1">
-        <v>283</v>
+        <v>294</v>
       </c>
       <c r="AK1" t="s" s="1">
-        <v>284</v>
+        <v>295</v>
       </c>
       <c r="AL1" t="s" s="1">
-        <v>285</v>
+        <v>296</v>
       </c>
       <c r="AM1" t="s" s="1">
-        <v>298</v>
+        <v>321</v>
       </c>
       <c r="AN1" t="s" s="1">
-        <v>299</v>
+        <v>322</v>
       </c>
       <c r="AO1" t="s" s="1">
-        <v>300</v>
+        <v>323</v>
       </c>
       <c r="AP1" t="s" s="1">
-        <v>306</v>
+        <v>329</v>
       </c>
       <c r="AQ1" t="s" s="1">
-        <v>307</v>
+        <v>330</v>
       </c>
       <c r="AR1" t="s" s="1">
-        <v>308</v>
+        <v>331</v>
       </c>
       <c r="AS1" t="s" s="1">
-        <v>315</v>
+        <v>338</v>
       </c>
       <c r="AT1" t="s" s="1">
-        <v>332</v>
+        <v>359</v>
       </c>
       <c r="AU1" t="s" s="1">
-        <v>333</v>
+        <v>360</v>
       </c>
     </row>
     <row r="2">
       <c r="AU2" t="s">
-        <v>334</v>
+        <v>361</v>
       </c>
     </row>
   </sheetData>
@@ -1741,7 +1822,7 @@
       <formula1>'acquisition_instrument_vendor'!$A$1:$A$14</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$32</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$36</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -1758,10 +1839,10 @@
       <formula1>'time_since_acquisition_instrument_calibration_unit'!$A$1:$A$3</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="O2:O1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'barcode_offset'!$A$1:$A$3</formula1>
+      <formula1>'barcode_offset'!$A$1:$A$4</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="P2:P1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'barcode_read'!$A$1:$A$2</formula1>
+      <formula1>'barcode_read'!$A$1:$A$3</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="Q2:Q1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'barcode_size'!$A$1:$A$6</formula1>
@@ -1818,7 +1899,7 @@
       <formula1>'library_preparation_kit'!$A$1:$A$6</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AH2:AH1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'sample_indexing_kit'!$A$1:$A$3</formula1>
+      <formula1>'sample_indexing_kit'!$A$1:$A$4</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AJ2:AJ1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'is_technical_replicate'!$A$1:$A$2</formula1>
@@ -1828,7 +1909,7 @@
       <formula2>2147483647</formula2>
     </dataValidation>
     <dataValidation type="list" sqref="AL2:AL1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'sequencing_reagent_kit'!$A$1:$A$6</formula1>
+      <formula1>'sequencing_reagent_kit'!$A$1:$A$12</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AN2:AN1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'transposition_reagent_kit'!$A$1:$A$3</formula1>
@@ -1837,10 +1918,10 @@
       <formula1>'transposition_method'!$A$1:$A$3</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AR2:AR1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'preparation_instrument_vendor'!$A$1:$A$5</formula1>
+      <formula1>'preparation_instrument_vendor'!$A$1:$A$7</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AS2:AS1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'preparation_instrument_model'!$A$1:$A$12</formula1>
+      <formula1>'preparation_instrument_model'!$A$1:$A$14</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AT2:AT1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'preparation_instrument_kit'!$A$1:$A$2</formula1>
@@ -1854,7 +1935,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1862,18 +1943,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>213</v>
+        <v>226</v>
       </c>
       <c r="B1" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="B2" t="s">
-        <v>219</v>
+        <v>228</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>229</v>
+      </c>
+      <c r="B3" t="s">
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -1891,32 +1980,32 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>221</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>222</v>
+        <v>233</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>223</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>224</v>
+        <v>235</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>225</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -1934,12 +2023,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>223</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -1957,26 +2046,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="B2" t="s">
-        <v>217</v>
+        <v>228</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>218</v>
+        <v>229</v>
       </c>
       <c r="B3" t="s">
-        <v>219</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -1994,27 +2083,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>233</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -2032,42 +2121,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
       <c r="B1" t="s">
-        <v>236</v>
+        <v>245</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>237</v>
+        <v>246</v>
       </c>
       <c r="B2" t="s">
-        <v>238</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>239</v>
+        <v>248</v>
       </c>
       <c r="B3" t="s">
-        <v>240</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>241</v>
+        <v>250</v>
       </c>
       <c r="B4" t="s">
-        <v>242</v>
+        <v>251</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>243</v>
+        <v>252</v>
       </c>
       <c r="B5" t="s">
-        <v>244</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -2085,10 +2174,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="B1" t="s">
-        <v>251</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -2106,10 +2195,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="B1" t="s">
-        <v>251</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -2127,10 +2216,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>256</v>
+        <v>265</v>
       </c>
       <c r="B1" t="s">
-        <v>257</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -2148,18 +2237,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>259</v>
+        <v>268</v>
       </c>
       <c r="B1" t="s">
-        <v>260</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>261</v>
+        <v>270</v>
       </c>
       <c r="B2" t="s">
-        <v>262</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -2478,50 +2567,50 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
       <c r="B1" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>267</v>
+        <v>276</v>
       </c>
       <c r="B2" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>269</v>
+        <v>278</v>
       </c>
       <c r="B3" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
       <c r="B4" t="s">
-        <v>272</v>
+        <v>281</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>273</v>
+        <v>282</v>
       </c>
       <c r="B5" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="B6" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -2531,7 +2620,7 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2539,26 +2628,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>278</v>
+        <v>287</v>
       </c>
       <c r="B1" t="s">
-        <v>279</v>
+        <v>288</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="B2" t="s">
-        <v>217</v>
+        <v>228</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>280</v>
+        <v>289</v>
       </c>
       <c r="B3" t="s">
-        <v>281</v>
+        <v>290</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>291</v>
+      </c>
+      <c r="B4" t="s">
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -2591,7 +2688,7 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2599,50 +2696,98 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>286</v>
+        <v>297</v>
       </c>
       <c r="B1" t="s">
-        <v>287</v>
+        <v>298</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>288</v>
+        <v>299</v>
       </c>
       <c r="B2" t="s">
-        <v>289</v>
+        <v>300</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>290</v>
+        <v>301</v>
       </c>
       <c r="B3" t="s">
-        <v>291</v>
+        <v>302</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>292</v>
+        <v>303</v>
       </c>
       <c r="B4" t="s">
-        <v>293</v>
+        <v>304</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>294</v>
+        <v>305</v>
       </c>
       <c r="B5" t="s">
-        <v>295</v>
+        <v>306</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>296</v>
+        <v>307</v>
       </c>
       <c r="B6" t="s">
-        <v>297</v>
+        <v>308</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>309</v>
+      </c>
+      <c r="B7" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>311</v>
+      </c>
+      <c r="B8" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>313</v>
+      </c>
+      <c r="B9" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>315</v>
+      </c>
+      <c r="B10" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>317</v>
+      </c>
+      <c r="B11" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>319</v>
+      </c>
+      <c r="B12" t="s">
+        <v>320</v>
       </c>
     </row>
   </sheetData>
@@ -2660,26 +2805,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
       <c r="B1" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>269</v>
+        <v>278</v>
       </c>
       <c r="B2" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="B3" t="s">
-        <v>217</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -2700,23 +2845,23 @@
         <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>301</v>
+        <v>324</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>302</v>
+        <v>325</v>
       </c>
       <c r="B2" t="s">
-        <v>303</v>
+        <v>326</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>304</v>
+        <v>327</v>
       </c>
       <c r="B3" t="s">
-        <v>305</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -2726,7 +2871,7 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2734,42 +2879,58 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>309</v>
+        <v>119</v>
       </c>
       <c r="B1" t="s">
-        <v>310</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>123</v>
+        <v>222</v>
       </c>
       <c r="B2" t="s">
-        <v>124</v>
+        <v>228</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>213</v>
+        <v>332</v>
       </c>
       <c r="B3" t="s">
-        <v>217</v>
+        <v>333</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>311</v>
+        <v>334</v>
       </c>
       <c r="B4" t="s">
-        <v>312</v>
+        <v>335</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>313</v>
+        <v>123</v>
       </c>
       <c r="B5" t="s">
-        <v>314</v>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>280</v>
+      </c>
+      <c r="B6" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>336</v>
+      </c>
+      <c r="B7" t="s">
+        <v>337</v>
       </c>
     </row>
   </sheetData>
@@ -2779,7 +2940,7 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2787,98 +2948,114 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>316</v>
+        <v>136</v>
       </c>
       <c r="B1" t="s">
-        <v>317</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>222</v>
       </c>
       <c r="B2" t="s">
-        <v>137</v>
+        <v>228</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>213</v>
+        <v>339</v>
       </c>
       <c r="B3" t="s">
-        <v>217</v>
+        <v>340</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>318</v>
+        <v>341</v>
       </c>
       <c r="B4" t="s">
-        <v>319</v>
+        <v>342</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>320</v>
+        <v>182</v>
       </c>
       <c r="B5" t="s">
-        <v>321</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>322</v>
+        <v>184</v>
       </c>
       <c r="B6" t="s">
-        <v>323</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>324</v>
+        <v>343</v>
       </c>
       <c r="B7" t="s">
-        <v>325</v>
+        <v>344</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>326</v>
+        <v>345</v>
       </c>
       <c r="B8" t="s">
-        <v>327</v>
+        <v>346</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>328</v>
+        <v>347</v>
       </c>
       <c r="B9" t="s">
-        <v>329</v>
+        <v>348</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>330</v>
+        <v>349</v>
       </c>
       <c r="B10" t="s">
-        <v>331</v>
+        <v>350</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>178</v>
+        <v>351</v>
       </c>
       <c r="B11" t="s">
-        <v>179</v>
+        <v>352</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>180</v>
+        <v>353</v>
       </c>
       <c r="B12" t="s">
-        <v>181</v>
+        <v>354</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>355</v>
+      </c>
+      <c r="B13" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>357</v>
+      </c>
+      <c r="B14" t="s">
+        <v>358</v>
       </c>
     </row>
   </sheetData>
@@ -2896,18 +3073,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
       <c r="B1" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>269</v>
+        <v>278</v>
       </c>
       <c r="B2" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -2931,30 +3108,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>335</v>
+        <v>362</v>
       </c>
       <c r="B1" t="s">
-        <v>337</v>
+        <v>364</v>
       </c>
       <c r="C1" t="s">
-        <v>339</v>
+        <v>366</v>
       </c>
       <c r="D1" t="s">
-        <v>341</v>
+        <v>368</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>336</v>
+        <v>363</v>
       </c>
       <c r="B2" t="s">
-        <v>338</v>
+        <v>365</v>
       </c>
       <c r="C2" t="s">
-        <v>340</v>
+        <v>367</v>
       </c>
       <c r="D2" t="s">
-        <v>342</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -3213,7 +3390,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3473,6 +3650,38 @@
       </c>
       <c r="B32" t="s">
         <v>195</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>196</v>
+      </c>
+      <c r="B33" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>198</v>
+      </c>
+      <c r="B34" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>200</v>
+      </c>
+      <c r="B35" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>202</v>
+      </c>
+      <c r="B36" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -3490,42 +3699,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="B1" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="B2" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="B3" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="B4" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="B5" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -3543,26 +3752,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="B1" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="B2" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="B3" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -3572,7 +3781,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3580,17 +3789,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>215</v>
+        <v>223</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating barcode_offset and umi_offset
</commit_message>
<xml_diff>
--- a/atacseq/latest/atacseq.xlsx
+++ b/atacseq/latest/atacseq.xlsx
@@ -381,7 +381,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="374">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -1046,7 +1046,7 @@
     <t>barcode_offset</t>
   </si>
   <si>
-    <t>0</t>
+    <t>0,38,76</t>
   </si>
   <si>
     <t>Not applicable</t>
@@ -1058,6 +1058,9 @@
     <t>8</t>
   </si>
   <si>
+    <t>10,48,86</t>
+  </si>
+  <si>
     <t>barcode_read</t>
   </si>
   <si>
@@ -1097,6 +1100,9 @@
     <t>umi_offset</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>umi_read</t>
   </si>
   <si>
@@ -1490,7 +1496,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2023-10-27T18:08:35-07:00</t>
+    <t>2023-10-31T13:53:10-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1713,105 +1719,105 @@
         <v>220</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="AD1" t="s" s="1">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="AE1" t="s" s="1">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="AF1" t="s" s="1">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="AG1" t="s" s="1">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="AH1" t="s" s="1">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="AI1" t="s" s="1">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="AJ1" t="s" s="1">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="AK1" t="s" s="1">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="AL1" t="s" s="1">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="AM1" t="s" s="1">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="AN1" t="s" s="1">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="AO1" t="s" s="1">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="AP1" t="s" s="1">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="AQ1" t="s" s="1">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="AR1" t="s" s="1">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="AS1" t="s" s="1">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="AT1" t="s" s="1">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="AU1" t="s" s="1">
-        <v>362</v>
+        <v>364</v>
       </c>
     </row>
     <row r="2">
       <c r="AU2" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
     </row>
   </sheetData>
@@ -1846,7 +1852,7 @@
       <formula1>'time_since_acquisition_instrument_calibration_unit'!$A$1:$A$3</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="O2:O1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'barcode_offset'!$A$1:$A$4</formula1>
+      <formula1>'barcode_offset'!$A$1:$A$5</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="P2:P1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'barcode_read'!$A$1:$A$3</formula1>
@@ -1855,7 +1861,7 @@
       <formula1>'barcode_size'!$A$1:$A$6</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="R2:R1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'umi_offset'!$A$1:$A$2</formula1>
+      <formula1>'umi_offset'!$A$1:$A$3</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="S2:S1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'umi_read'!$A$1:$A$3</formula1>
@@ -1950,10 +1956,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="2">
@@ -1961,15 +1967,15 @@
         <v>222</v>
       </c>
       <c r="B2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B3" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -1987,12 +1993,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3">
@@ -2002,17 +2008,17 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -2022,7 +2028,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2030,12 +2036,17 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>222</v>
+        <v>239</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>234</v>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -2053,10 +2064,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="2">
@@ -2064,15 +2075,15 @@
         <v>222</v>
       </c>
       <c r="B2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B3" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -2090,7 +2101,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="2">
@@ -2105,12 +2116,12 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -2128,42 +2139,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B1" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B2" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B3" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B4" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B5" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -2181,10 +2192,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B1" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -2202,10 +2213,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B1" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -2223,10 +2234,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="B1" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -2244,18 +2255,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B1" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B2" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -2574,50 +2585,50 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B1" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B2" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B3" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B4" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B5" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B6" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -2635,10 +2646,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B1" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="2">
@@ -2646,23 +2657,23 @@
         <v>222</v>
       </c>
       <c r="B2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B3" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B4" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
   </sheetData>
@@ -2703,98 +2714,98 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="B1" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="B2" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="B3" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="B4" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="B5" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="B6" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="B7" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="B8" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="B9" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="B10" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B11" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B12" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
   </sheetData>
@@ -2812,18 +2823,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B1" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B2" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="3">
@@ -2831,7 +2842,7 @@
         <v>222</v>
       </c>
       <c r="B3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -2852,23 +2863,23 @@
         <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B2" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B3" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -2886,10 +2897,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="B1" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row r="2">
@@ -2905,23 +2916,23 @@
         <v>222</v>
       </c>
       <c r="B3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="B4" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="B5" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
     </row>
     <row r="6">
@@ -2934,10 +2945,10 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="B7" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
     </row>
   </sheetData>
@@ -2966,23 +2977,23 @@
         <v>222</v>
       </c>
       <c r="B2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="B3" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="B4" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
     </row>
     <row r="5">
@@ -3003,66 +3014,66 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="B7" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="B8" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B9" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="B10" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="B11" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B12" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B13" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="B14" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -3080,18 +3091,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B1" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B2" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -3115,30 +3126,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="B1" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="C1" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="D1" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="B2" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="C2" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="D2" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
     </row>
   </sheetData>
@@ -3788,7 +3799,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3814,6 +3825,11 @@
         <v>224</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>225</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Added 0 as an alternative option for barcode_offset
</commit_message>
<xml_diff>
--- a/atacseq/latest/atacseq.xlsx
+++ b/atacseq/latest/atacseq.xlsx
@@ -381,7 +381,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="375">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -1046,6 +1046,9 @@
     <t>barcode_offset</t>
   </si>
   <si>
+    <t>0</t>
+  </si>
+  <si>
     <t>0,38,76</t>
   </si>
   <si>
@@ -1496,7 +1499,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2023-10-31T13:53:10-07:00</t>
+    <t>2023-10-31T14:33:15-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1719,105 +1722,105 @@
         <v>220</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AD1" t="s" s="1">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="AE1" t="s" s="1">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="AF1" t="s" s="1">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="AG1" t="s" s="1">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="AH1" t="s" s="1">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="AI1" t="s" s="1">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="AJ1" t="s" s="1">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="AK1" t="s" s="1">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="AL1" t="s" s="1">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="AM1" t="s" s="1">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="AN1" t="s" s="1">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="AO1" t="s" s="1">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="AP1" t="s" s="1">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="AQ1" t="s" s="1">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="AR1" t="s" s="1">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="AS1" t="s" s="1">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="AT1" t="s" s="1">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="AU1" t="s" s="1">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="2">
       <c r="AU2" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -1852,7 +1855,7 @@
       <formula1>'time_since_acquisition_instrument_calibration_unit'!$A$1:$A$3</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="O2:O1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'barcode_offset'!$A$1:$A$5</formula1>
+      <formula1>'barcode_offset'!$A$1:$A$6</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="P2:P1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'barcode_read'!$A$1:$A$3</formula1>
@@ -1956,26 +1959,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -1993,32 +1996,32 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -2036,17 +2039,17 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -2064,26 +2067,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -2101,27 +2104,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -2139,42 +2142,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B3" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B4" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B5" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -2192,10 +2195,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -2213,10 +2216,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -2234,10 +2237,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -2255,18 +2258,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -2585,50 +2588,50 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B2" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B3" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B4" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B5" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
   </sheetData>
@@ -2646,34 +2649,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B3" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B4" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
   </sheetData>
@@ -2714,98 +2717,98 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B2" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B3" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B4" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B5" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B6" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B7" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B8" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B9" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B10" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B11" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B12" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
   </sheetData>
@@ -2823,26 +2826,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B2" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -2863,23 +2866,23 @@
         <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B2" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B3" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
   </sheetData>
@@ -2897,10 +2900,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B1" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="2">
@@ -2913,26 +2916,26 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B4" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B5" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="6">
@@ -2945,10 +2948,10 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B7" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
   </sheetData>
@@ -2974,26 +2977,26 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B3" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B4" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="5">
@@ -3014,66 +3017,66 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B7" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B8" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B9" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B10" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B11" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B12" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B13" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B14" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
   </sheetData>
@@ -3091,18 +3094,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B2" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -3126,30 +3129,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C1" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="D1" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B2" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C2" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D2" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
   </sheetData>
@@ -3799,7 +3802,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3830,6 +3833,11 @@
         <v>225</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>226</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Roll back umi_offset permissible values
</commit_message>
<xml_diff>
--- a/atacseq/latest/atacseq.xlsx
+++ b/atacseq/latest/atacseq.xlsx
@@ -381,7 +381,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="374">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -1103,9 +1103,6 @@
     <t>umi_offset</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>umi_read</t>
   </si>
   <si>
@@ -1499,7 +1496,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2023-10-31T14:33:15-07:00</t>
+    <t>2023-11-01T15:15:54-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1731,96 +1728,96 @@
         <v>239</v>
       </c>
       <c r="S1" t="s" s="1">
+        <v>240</v>
+      </c>
+      <c r="T1" t="s" s="1">
         <v>241</v>
       </c>
-      <c r="T1" t="s" s="1">
-        <v>242</v>
-      </c>
       <c r="U1" t="s" s="1">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="V1" t="s" s="1">
+        <v>256</v>
+      </c>
+      <c r="W1" t="s" s="1">
         <v>257</v>
       </c>
-      <c r="W1" t="s" s="1">
+      <c r="X1" t="s" s="1">
         <v>258</v>
       </c>
-      <c r="X1" t="s" s="1">
+      <c r="Y1" t="s" s="1">
         <v>259</v>
       </c>
-      <c r="Y1" t="s" s="1">
+      <c r="Z1" t="s" s="1">
         <v>260</v>
       </c>
-      <c r="Z1" t="s" s="1">
-        <v>261</v>
-      </c>
       <c r="AA1" t="s" s="1">
+        <v>263</v>
+      </c>
+      <c r="AB1" t="s" s="1">
         <v>264</v>
       </c>
-      <c r="AB1" t="s" s="1">
+      <c r="AC1" t="s" s="1">
         <v>265</v>
       </c>
-      <c r="AC1" t="s" s="1">
+      <c r="AD1" t="s" s="1">
         <v>266</v>
       </c>
-      <c r="AD1" t="s" s="1">
-        <v>267</v>
-      </c>
       <c r="AE1" t="s" s="1">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="AF1" t="s" s="1">
+        <v>274</v>
+      </c>
+      <c r="AG1" t="s" s="1">
         <v>275</v>
       </c>
-      <c r="AG1" t="s" s="1">
-        <v>276</v>
-      </c>
       <c r="AH1" t="s" s="1">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="AI1" t="s" s="1">
+        <v>295</v>
+      </c>
+      <c r="AJ1" t="s" s="1">
         <v>296</v>
       </c>
-      <c r="AJ1" t="s" s="1">
+      <c r="AK1" t="s" s="1">
         <v>297</v>
       </c>
-      <c r="AK1" t="s" s="1">
+      <c r="AL1" t="s" s="1">
         <v>298</v>
       </c>
-      <c r="AL1" t="s" s="1">
-        <v>299</v>
-      </c>
       <c r="AM1" t="s" s="1">
+        <v>323</v>
+      </c>
+      <c r="AN1" t="s" s="1">
         <v>324</v>
       </c>
-      <c r="AN1" t="s" s="1">
+      <c r="AO1" t="s" s="1">
         <v>325</v>
       </c>
-      <c r="AO1" t="s" s="1">
-        <v>326</v>
-      </c>
       <c r="AP1" t="s" s="1">
+        <v>331</v>
+      </c>
+      <c r="AQ1" t="s" s="1">
         <v>332</v>
       </c>
-      <c r="AQ1" t="s" s="1">
+      <c r="AR1" t="s" s="1">
         <v>333</v>
       </c>
-      <c r="AR1" t="s" s="1">
-        <v>334</v>
-      </c>
       <c r="AS1" t="s" s="1">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="AT1" t="s" s="1">
+        <v>363</v>
+      </c>
+      <c r="AU1" t="s" s="1">
         <v>364</v>
-      </c>
-      <c r="AU1" t="s" s="1">
-        <v>365</v>
       </c>
     </row>
     <row r="2">
       <c r="AU2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
   </sheetData>
@@ -1864,7 +1861,7 @@
       <formula1>'barcode_size'!$A$1:$A$6</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="R2:R1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'umi_offset'!$A$1:$A$3</formula1>
+      <formula1>'umi_offset'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="S2:S1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'umi_read'!$A$1:$A$3</formula1>
@@ -2031,7 +2028,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2039,16 +2036,11 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
         <v>236</v>
       </c>
     </row>
@@ -2104,7 +2096,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="2">
@@ -2119,12 +2111,12 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -2142,42 +2134,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B1" t="s">
         <v>247</v>
-      </c>
-      <c r="B1" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B2" t="s">
         <v>249</v>
-      </c>
-      <c r="B2" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>250</v>
+      </c>
+      <c r="B3" t="s">
         <v>251</v>
-      </c>
-      <c r="B3" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>252</v>
+      </c>
+      <c r="B4" t="s">
         <v>253</v>
-      </c>
-      <c r="B4" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>254</v>
+      </c>
+      <c r="B5" t="s">
         <v>255</v>
-      </c>
-      <c r="B5" t="s">
-        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -2195,10 +2187,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B1" t="s">
         <v>262</v>
-      </c>
-      <c r="B1" t="s">
-        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -2216,10 +2208,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B1" t="s">
         <v>262</v>
-      </c>
-      <c r="B1" t="s">
-        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -2237,10 +2229,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B1" t="s">
         <v>268</v>
-      </c>
-      <c r="B1" t="s">
-        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -2258,18 +2250,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B1" t="s">
         <v>271</v>
-      </c>
-      <c r="B1" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B2" t="s">
         <v>273</v>
-      </c>
-      <c r="B2" t="s">
-        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -2588,50 +2580,50 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B1" t="s">
         <v>277</v>
-      </c>
-      <c r="B1" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B2" t="s">
         <v>279</v>
-      </c>
-      <c r="B2" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>280</v>
+      </c>
+      <c r="B3" t="s">
         <v>281</v>
-      </c>
-      <c r="B3" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>282</v>
+      </c>
+      <c r="B4" t="s">
         <v>283</v>
-      </c>
-      <c r="B4" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B5" t="s">
         <v>285</v>
-      </c>
-      <c r="B5" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>286</v>
+      </c>
+      <c r="B6" t="s">
         <v>287</v>
-      </c>
-      <c r="B6" t="s">
-        <v>288</v>
       </c>
     </row>
   </sheetData>
@@ -2649,10 +2641,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B1" t="s">
         <v>290</v>
-      </c>
-      <c r="B1" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="2">
@@ -2665,18 +2657,18 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>291</v>
+      </c>
+      <c r="B3" t="s">
         <v>292</v>
-      </c>
-      <c r="B3" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B4" t="s">
         <v>294</v>
-      </c>
-      <c r="B4" t="s">
-        <v>295</v>
       </c>
     </row>
   </sheetData>
@@ -2717,98 +2709,98 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B1" t="s">
         <v>300</v>
-      </c>
-      <c r="B1" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2" t="s">
         <v>302</v>
-      </c>
-      <c r="B2" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>303</v>
+      </c>
+      <c r="B3" t="s">
         <v>304</v>
-      </c>
-      <c r="B3" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>305</v>
+      </c>
+      <c r="B4" t="s">
         <v>306</v>
-      </c>
-      <c r="B4" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>307</v>
+      </c>
+      <c r="B5" t="s">
         <v>308</v>
-      </c>
-      <c r="B5" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>309</v>
+      </c>
+      <c r="B6" t="s">
         <v>310</v>
-      </c>
-      <c r="B6" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>311</v>
+      </c>
+      <c r="B7" t="s">
         <v>312</v>
-      </c>
-      <c r="B7" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>313</v>
+      </c>
+      <c r="B8" t="s">
         <v>314</v>
-      </c>
-      <c r="B8" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>315</v>
+      </c>
+      <c r="B9" t="s">
         <v>316</v>
-      </c>
-      <c r="B9" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
+        <v>317</v>
+      </c>
+      <c r="B10" t="s">
         <v>318</v>
-      </c>
-      <c r="B10" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
+        <v>319</v>
+      </c>
+      <c r="B11" t="s">
         <v>320</v>
-      </c>
-      <c r="B11" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>321</v>
+      </c>
+      <c r="B12" t="s">
         <v>322</v>
-      </c>
-      <c r="B12" t="s">
-        <v>323</v>
       </c>
     </row>
   </sheetData>
@@ -2826,18 +2818,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B1" t="s">
         <v>277</v>
-      </c>
-      <c r="B1" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B2" t="s">
         <v>281</v>
-      </c>
-      <c r="B2" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="3">
@@ -2866,23 +2858,23 @@
         <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>327</v>
+      </c>
+      <c r="B2" t="s">
         <v>328</v>
-      </c>
-      <c r="B2" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>329</v>
+      </c>
+      <c r="B3" t="s">
         <v>330</v>
-      </c>
-      <c r="B3" t="s">
-        <v>331</v>
       </c>
     </row>
   </sheetData>
@@ -2900,10 +2892,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B1" t="s">
         <v>335</v>
-      </c>
-      <c r="B1" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="2">
@@ -2924,18 +2916,18 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>336</v>
+      </c>
+      <c r="B4" t="s">
         <v>337</v>
-      </c>
-      <c r="B4" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>338</v>
+      </c>
+      <c r="B5" t="s">
         <v>339</v>
-      </c>
-      <c r="B5" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="6">
@@ -2948,10 +2940,10 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>340</v>
+      </c>
+      <c r="B7" t="s">
         <v>341</v>
-      </c>
-      <c r="B7" t="s">
-        <v>342</v>
       </c>
     </row>
   </sheetData>
@@ -2985,18 +2977,18 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>343</v>
+      </c>
+      <c r="B3" t="s">
         <v>344</v>
-      </c>
-      <c r="B3" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>345</v>
+      </c>
+      <c r="B4" t="s">
         <v>346</v>
-      </c>
-      <c r="B4" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="5">
@@ -3017,66 +3009,66 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>347</v>
+      </c>
+      <c r="B7" t="s">
         <v>348</v>
-      </c>
-      <c r="B7" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>349</v>
+      </c>
+      <c r="B8" t="s">
         <v>350</v>
-      </c>
-      <c r="B8" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>351</v>
+      </c>
+      <c r="B9" t="s">
         <v>352</v>
-      </c>
-      <c r="B9" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
+        <v>353</v>
+      </c>
+      <c r="B10" t="s">
         <v>354</v>
-      </c>
-      <c r="B10" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
+        <v>355</v>
+      </c>
+      <c r="B11" t="s">
         <v>356</v>
-      </c>
-      <c r="B11" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>357</v>
+      </c>
+      <c r="B12" t="s">
         <v>358</v>
-      </c>
-      <c r="B12" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
+        <v>359</v>
+      </c>
+      <c r="B13" t="s">
         <v>360</v>
-      </c>
-      <c r="B13" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
+        <v>361</v>
+      </c>
+      <c r="B14" t="s">
         <v>362</v>
-      </c>
-      <c r="B14" t="s">
-        <v>363</v>
       </c>
     </row>
   </sheetData>
@@ -3094,18 +3086,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B1" t="s">
         <v>277</v>
-      </c>
-      <c r="B1" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B2" t="s">
         <v>281</v>
-      </c>
-      <c r="B2" t="s">
-        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -3129,30 +3121,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a new sequencing reagent kit
</commit_message>
<xml_diff>
--- a/atacseq/latest/atacseq.xlsx
+++ b/atacseq/latest/atacseq.xlsx
@@ -381,7 +381,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="378">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -395,6 +395,12 @@
     <t>dataset_type</t>
   </si>
   <si>
+    <t>HiFi-Slide</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000195</t>
+  </si>
+  <si>
     <t>SNARE-seq2</t>
   </si>
   <si>
@@ -515,12 +521,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000309</t>
   </si>
   <si>
-    <t>HiFi-Slides</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000195</t>
-  </si>
-  <si>
     <t>Histology</t>
   </si>
   <si>
@@ -1286,60 +1286,72 @@
     <t>sequencing_reagent_kit</t>
   </si>
   <si>
+    <t>Illumina; NovaSeq X Series 1.5B Reagent Kit (100 Cycle); PN 20104703</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000286</t>
+  </si>
+  <si>
+    <t>Illumina; NovaSeq X Series 1.5B Reagent Kit (300 Cycle); PN 20104705</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000288</t>
+  </si>
+  <si>
+    <t>Illumina; NovaSeq 6000 S1 Reagent v1.5 Kit (100 Cycles); PN 20028319</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000257</t>
+  </si>
+  <si>
+    <t>Illumina; NovaSeq 6000 SP Reagent v1.5 Kit (100 Cycles); PN 20028401</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000256</t>
+  </si>
+  <si>
+    <t>Illumina; HiSeq 3000/4000 PE Cluster Kit PE-410-1001; PN 1000283</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000254</t>
+  </si>
+  <si>
+    <t>Illumina; NovaSeq X Series 10B Reagent Kit (200 Cycle); PN 20085595</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000284</t>
+  </si>
+  <si>
+    <t>Illumina; NextSeq 500/550 Hi Output Kit 150 Cycles; v2.5; PN 20024907</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000255</t>
+  </si>
+  <si>
+    <t>Illumina; NovaSeq 6000 S1 Reagent Kit (200 Cycles); PN 20012864</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000313</t>
+  </si>
+  <si>
     <t>Illumina; NovaSeq 6000 S4 Reagent v1.5 Kit (200 Cycles); PN 20028313</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000259</t>
   </si>
   <si>
-    <t>Illumina; NovaSeq X Series 1.5B Reagent Kit (100 Cycle); PN 20104703</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000286</t>
-  </si>
-  <si>
-    <t>Illumina; NovaSeq X Series 1.5B Reagent Kit (300 Cycle); PN 20104705</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000288</t>
-  </si>
-  <si>
-    <t>Illumina; NovaSeq 6000 S1 Reagent v1.5 Kit (100 Cycles); PN 20028319</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000257</t>
-  </si>
-  <si>
     <t>Illumina; NovaSeq X Series 1.5B Reagent Kit (200 Cycle); PN 20104704</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000287</t>
   </si>
   <si>
-    <t>Illumina; NovaSeq 6000 SP Reagent v1.5 Kit (100 Cycles); PN 20028401</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000256</t>
-  </si>
-  <si>
-    <t>Illumina; HiSeq 3000/4000 PE Cluster Kit PE-410-1001; PN 1000283</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000254</t>
-  </si>
-  <si>
     <t>Illumina; NovaSeq X Series 10B Reagent Kit (300 Cycle); PN 20085594</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000283</t>
   </si>
   <si>
-    <t>Illumina; NovaSeq X Series 10B Reagent Kit (200 Cycle); PN 20085595</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000284</t>
-  </si>
-  <si>
     <t>Illumina; NovaSeq X Series 10B Reagent Kit (100 Cycle); PN 20085596</t>
   </si>
   <si>
@@ -1352,12 +1364,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000258</t>
   </si>
   <si>
-    <t>Illumina; NextSeq 500/550 Hi Output Kit 150 Cycles; v2.5; PN 20024907</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000255</t>
-  </si>
-  <si>
     <t>sequencing_read_format</t>
   </si>
   <si>
@@ -1502,7 +1508,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2023-11-22T10:20:08-08:00</t>
+    <t>2023-11-24T09:44:59-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1794,39 +1800,39 @@
         <v>300</v>
       </c>
       <c r="AM1" t="s" s="1">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="AN1" t="s" s="1">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="AO1" t="s" s="1">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="AP1" t="s" s="1">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="AQ1" t="s" s="1">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="AR1" t="s" s="1">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="AS1" t="s" s="1">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="AT1" t="s" s="1">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="AU1" t="s" s="1">
-        <v>367</v>
+        <v>369</v>
       </c>
     </row>
     <row r="2">
       <c r="D2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="AU2" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
   </sheetData>
@@ -1931,7 +1937,7 @@
       <formula2>2147483647</formula2>
     </dataValidation>
     <dataValidation type="list" sqref="AL2:AL1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'sequencing_reagent_kit'!$A$1:$A$12</formula1>
+      <formula1>'sequencing_reagent_kit'!$A$1:$A$13</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AN2:AN1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'transposition_reagent_kit'!$A$1:$A$3</formula1>
@@ -2707,7 +2713,7 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2807,6 +2813,14 @@
       </c>
       <c r="B12" t="s">
         <v>324</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>325</v>
+      </c>
+      <c r="B13" t="s">
+        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -2861,26 +2875,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="B1" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="B2" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="B3" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
   </sheetData>
@@ -2898,10 +2912,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="B1" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="2">
@@ -2922,18 +2936,18 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="B4" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="B5" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
     </row>
     <row r="6">
@@ -2946,10 +2960,10 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="B7" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
     </row>
   </sheetData>
@@ -2983,18 +2997,18 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="B3" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="B4" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
     </row>
     <row r="5">
@@ -3015,66 +3029,66 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="B7" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="B8" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="B9" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="B10" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="B11" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="B12" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="B13" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="B14" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
   </sheetData>
@@ -3127,30 +3141,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="B1" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="C1" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="D1" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="C2" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="D2" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new acquisition instrument vendors and models
</commit_message>
<xml_diff>
--- a/atacseq/latest/atacseq.xlsx
+++ b/atacseq/latest/atacseq.xlsx
@@ -381,7 +381,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="392">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -674,6 +674,12 @@
     <t>acquisition_instrument_vendor</t>
   </si>
   <si>
+    <t>BGI Genomics</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024848</t>
+  </si>
+  <si>
     <t>Resolve Biosciences</t>
   </si>
   <si>
@@ -716,6 +722,12 @@
     <t>https://identifiers.org/RRID:SCR_017365</t>
   </si>
   <si>
+    <t>Evident Scientific (Olympus)</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024782</t>
+  </si>
+  <si>
     <t>Keyence</t>
   </si>
   <si>
@@ -752,6 +764,12 @@
     <t>https://identifiers.org/RRID:SCR_010233</t>
   </si>
   <si>
+    <t>Motic</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024856</t>
+  </si>
+  <si>
     <t>Ionpath</t>
   </si>
   <si>
@@ -785,6 +803,12 @@
     <t>https://identifiers.org/RRID:SCR_023760</t>
   </si>
   <si>
+    <t>MoticEasyScan One</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024855</t>
+  </si>
+  <si>
     <t>Axio Observer 7</t>
   </si>
   <si>
@@ -803,6 +827,12 @@
     <t>https://identifiers.org/RRID:SCR_023616</t>
   </si>
   <si>
+    <t>DM6 B</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024857</t>
+  </si>
+  <si>
     <t>NanoZoomer 2.0-HT</t>
   </si>
   <si>
@@ -815,6 +845,12 @@
     <t>https://identifiers.org/RRID:SCR_024448</t>
   </si>
   <si>
+    <t>DNBSEQ-T7</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024847</t>
+  </si>
+  <si>
     <t>Orbitrap Fusion Lumos Tribrid</t>
   </si>
   <si>
@@ -839,6 +875,12 @@
     <t>https://identifiers.org/RRID:SCR_023615</t>
   </si>
   <si>
+    <t>VS200 Slide Scanner</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024783</t>
+  </si>
+  <si>
     <t>Axio Observer 5</t>
   </si>
   <si>
@@ -1508,7 +1550,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2023-11-24T09:44:59-08:00</t>
+    <t>2024-01-09T21:21:27-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1707,124 +1749,124 @@
         <v>96</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>203</v>
+        <v>217</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>214</v>
+        <v>228</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>215</v>
+        <v>229</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>216</v>
+        <v>230</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>217</v>
+        <v>231</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>218</v>
+        <v>232</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>225</v>
+        <v>239</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>231</v>
+        <v>245</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>237</v>
+        <v>251</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>238</v>
+        <v>252</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>239</v>
+        <v>253</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>243</v>
+        <v>257</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>254</v>
+        <v>268</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>255</v>
+        <v>269</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>256</v>
+        <v>270</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>257</v>
+        <v>271</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>258</v>
+        <v>272</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>261</v>
+        <v>275</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>262</v>
+        <v>276</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>263</v>
+        <v>277</v>
       </c>
       <c r="AD1" t="s" s="1">
-        <v>264</v>
+        <v>278</v>
       </c>
       <c r="AE1" t="s" s="1">
-        <v>269</v>
+        <v>283</v>
       </c>
       <c r="AF1" t="s" s="1">
-        <v>274</v>
+        <v>288</v>
       </c>
       <c r="AG1" t="s" s="1">
-        <v>275</v>
+        <v>289</v>
       </c>
       <c r="AH1" t="s" s="1">
-        <v>290</v>
+        <v>304</v>
       </c>
       <c r="AI1" t="s" s="1">
-        <v>297</v>
+        <v>311</v>
       </c>
       <c r="AJ1" t="s" s="1">
-        <v>298</v>
+        <v>312</v>
       </c>
       <c r="AK1" t="s" s="1">
-        <v>299</v>
+        <v>313</v>
       </c>
       <c r="AL1" t="s" s="1">
-        <v>300</v>
+        <v>314</v>
       </c>
       <c r="AM1" t="s" s="1">
-        <v>327</v>
+        <v>341</v>
       </c>
       <c r="AN1" t="s" s="1">
-        <v>328</v>
+        <v>342</v>
       </c>
       <c r="AO1" t="s" s="1">
-        <v>329</v>
+        <v>343</v>
       </c>
       <c r="AP1" t="s" s="1">
-        <v>336</v>
+        <v>350</v>
       </c>
       <c r="AQ1" t="s" s="1">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="AR1" t="s" s="1">
-        <v>338</v>
+        <v>352</v>
       </c>
       <c r="AS1" t="s" s="1">
-        <v>347</v>
+        <v>361</v>
       </c>
       <c r="AT1" t="s" s="1">
-        <v>368</v>
+        <v>382</v>
       </c>
       <c r="AU1" t="s" s="1">
-        <v>369</v>
+        <v>383</v>
       </c>
     </row>
     <row r="2">
@@ -1832,7 +1874,7 @@
         <v>44</v>
       </c>
       <c r="AU2" t="s">
-        <v>370</v>
+        <v>384</v>
       </c>
     </row>
   </sheetData>
@@ -1847,10 +1889,10 @@
       <formula1>'is_targeted'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_vendor'!$A$1:$A$14</formula1>
+      <formula1>'acquisition_instrument_vendor'!$A$1:$A$17</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$38</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$42</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -1971,26 +2013,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>226</v>
+        <v>240</v>
       </c>
       <c r="B1" t="s">
-        <v>227</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>221</v>
+        <v>235</v>
       </c>
       <c r="B2" t="s">
-        <v>228</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>229</v>
+        <v>243</v>
       </c>
       <c r="B3" t="s">
-        <v>230</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -2008,32 +2050,32 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>232</v>
+        <v>246</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>233</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>221</v>
+        <v>235</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>234</v>
+        <v>248</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>235</v>
+        <v>249</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>236</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -2051,17 +2093,17 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>219</v>
+        <v>233</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>221</v>
+        <v>235</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>234</v>
+        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -2079,26 +2121,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>226</v>
+        <v>240</v>
       </c>
       <c r="B1" t="s">
-        <v>227</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>221</v>
+        <v>235</v>
       </c>
       <c r="B2" t="s">
-        <v>228</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>229</v>
+        <v>243</v>
       </c>
       <c r="B3" t="s">
-        <v>230</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -2116,27 +2158,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>240</v>
+        <v>254</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>221</v>
+        <v>235</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>223</v>
+        <v>237</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>241</v>
+        <v>255</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>242</v>
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -2154,42 +2196,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>244</v>
+        <v>258</v>
       </c>
       <c r="B1" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>246</v>
+        <v>260</v>
       </c>
       <c r="B2" t="s">
-        <v>247</v>
+        <v>261</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>248</v>
+        <v>262</v>
       </c>
       <c r="B3" t="s">
-        <v>249</v>
+        <v>263</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>250</v>
+        <v>264</v>
       </c>
       <c r="B4" t="s">
-        <v>251</v>
+        <v>265</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>252</v>
+        <v>266</v>
       </c>
       <c r="B5" t="s">
-        <v>253</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -2207,10 +2249,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>259</v>
+        <v>273</v>
       </c>
       <c r="B1" t="s">
-        <v>260</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -2228,10 +2270,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>259</v>
+        <v>273</v>
       </c>
       <c r="B1" t="s">
-        <v>260</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -2249,18 +2291,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>265</v>
+        <v>279</v>
       </c>
       <c r="B1" t="s">
-        <v>266</v>
+        <v>280</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>267</v>
+        <v>281</v>
       </c>
       <c r="B2" t="s">
-        <v>268</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -2278,18 +2320,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>270</v>
+        <v>284</v>
       </c>
       <c r="B1" t="s">
-        <v>271</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>272</v>
+        <v>286</v>
       </c>
       <c r="B2" t="s">
-        <v>273</v>
+        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -2584,58 +2626,58 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>276</v>
+        <v>290</v>
       </c>
       <c r="B1" t="s">
-        <v>277</v>
+        <v>291</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>278</v>
+        <v>292</v>
       </c>
       <c r="B2" t="s">
-        <v>279</v>
+        <v>293</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>280</v>
+        <v>294</v>
       </c>
       <c r="B3" t="s">
-        <v>281</v>
+        <v>295</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>282</v>
+        <v>296</v>
       </c>
       <c r="B4" t="s">
-        <v>283</v>
+        <v>297</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>284</v>
+        <v>298</v>
       </c>
       <c r="B5" t="s">
-        <v>285</v>
+        <v>299</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>286</v>
+        <v>300</v>
       </c>
       <c r="B6" t="s">
-        <v>287</v>
+        <v>301</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>288</v>
+        <v>302</v>
       </c>
       <c r="B7" t="s">
-        <v>289</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -2653,34 +2695,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>291</v>
+        <v>305</v>
       </c>
       <c r="B1" t="s">
-        <v>292</v>
+        <v>306</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>221</v>
+        <v>235</v>
       </c>
       <c r="B2" t="s">
-        <v>228</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>293</v>
+        <v>307</v>
       </c>
       <c r="B3" t="s">
-        <v>294</v>
+        <v>308</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>295</v>
+        <v>309</v>
       </c>
       <c r="B4" t="s">
-        <v>296</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>
@@ -2721,106 +2763,106 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>301</v>
+        <v>315</v>
       </c>
       <c r="B1" t="s">
-        <v>302</v>
+        <v>316</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>303</v>
+        <v>317</v>
       </c>
       <c r="B2" t="s">
-        <v>304</v>
+        <v>318</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>305</v>
+        <v>319</v>
       </c>
       <c r="B3" t="s">
-        <v>306</v>
+        <v>320</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>307</v>
+        <v>321</v>
       </c>
       <c r="B4" t="s">
-        <v>308</v>
+        <v>322</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>309</v>
+        <v>323</v>
       </c>
       <c r="B5" t="s">
-        <v>310</v>
+        <v>324</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>311</v>
+        <v>325</v>
       </c>
       <c r="B6" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>313</v>
+        <v>327</v>
       </c>
       <c r="B7" t="s">
-        <v>314</v>
+        <v>328</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>315</v>
+        <v>329</v>
       </c>
       <c r="B8" t="s">
-        <v>316</v>
+        <v>330</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>317</v>
+        <v>331</v>
       </c>
       <c r="B9" t="s">
-        <v>318</v>
+        <v>332</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>319</v>
+        <v>333</v>
       </c>
       <c r="B10" t="s">
-        <v>320</v>
+        <v>334</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>321</v>
+        <v>335</v>
       </c>
       <c r="B11" t="s">
-        <v>322</v>
+        <v>336</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>323</v>
+        <v>337</v>
       </c>
       <c r="B12" t="s">
-        <v>324</v>
+        <v>338</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>325</v>
+        <v>339</v>
       </c>
       <c r="B13" t="s">
-        <v>326</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>
@@ -2838,26 +2880,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>280</v>
+        <v>294</v>
       </c>
       <c r="B1" t="s">
-        <v>281</v>
+        <v>295</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>276</v>
+        <v>290</v>
       </c>
       <c r="B2" t="s">
-        <v>277</v>
+        <v>291</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>221</v>
+        <v>235</v>
       </c>
       <c r="B3" t="s">
-        <v>228</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -2875,26 +2917,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="B1" t="s">
-        <v>331</v>
+        <v>345</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>332</v>
+        <v>346</v>
       </c>
       <c r="B2" t="s">
-        <v>333</v>
+        <v>347</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>334</v>
+        <v>348</v>
       </c>
       <c r="B3" t="s">
-        <v>335</v>
+        <v>349</v>
       </c>
     </row>
   </sheetData>
@@ -2912,58 +2954,58 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>339</v>
+        <v>353</v>
       </c>
       <c r="B1" t="s">
-        <v>340</v>
+        <v>354</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B2" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>221</v>
+        <v>235</v>
       </c>
       <c r="B3" t="s">
-        <v>228</v>
+        <v>242</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>341</v>
+        <v>355</v>
       </c>
       <c r="B4" t="s">
-        <v>342</v>
+        <v>356</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>343</v>
+        <v>357</v>
       </c>
       <c r="B5" t="s">
-        <v>344</v>
+        <v>358</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B6" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>345</v>
+        <v>359</v>
       </c>
       <c r="B7" t="s">
-        <v>346</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -2981,114 +3023,114 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="B1" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>221</v>
+        <v>235</v>
       </c>
       <c r="B2" t="s">
-        <v>228</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>348</v>
+        <v>362</v>
       </c>
       <c r="B3" t="s">
-        <v>349</v>
+        <v>363</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>350</v>
+        <v>364</v>
       </c>
       <c r="B4" t="s">
-        <v>351</v>
+        <v>365</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>180</v>
+        <v>194</v>
       </c>
       <c r="B5" t="s">
-        <v>181</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>182</v>
+        <v>196</v>
       </c>
       <c r="B6" t="s">
-        <v>183</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>352</v>
+        <v>366</v>
       </c>
       <c r="B7" t="s">
-        <v>353</v>
+        <v>367</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>354</v>
+        <v>368</v>
       </c>
       <c r="B8" t="s">
-        <v>355</v>
+        <v>369</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>356</v>
+        <v>370</v>
       </c>
       <c r="B9" t="s">
-        <v>357</v>
+        <v>371</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>358</v>
+        <v>372</v>
       </c>
       <c r="B10" t="s">
-        <v>359</v>
+        <v>373</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>360</v>
+        <v>374</v>
       </c>
       <c r="B11" t="s">
-        <v>361</v>
+        <v>375</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>362</v>
+        <v>376</v>
       </c>
       <c r="B12" t="s">
-        <v>363</v>
+        <v>377</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>364</v>
+        <v>378</v>
       </c>
       <c r="B13" t="s">
-        <v>365</v>
+        <v>379</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>366</v>
+        <v>380</v>
       </c>
       <c r="B14" t="s">
-        <v>367</v>
+        <v>381</v>
       </c>
     </row>
   </sheetData>
@@ -3106,18 +3148,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>280</v>
+        <v>294</v>
       </c>
       <c r="B1" t="s">
-        <v>281</v>
+        <v>295</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>276</v>
+        <v>290</v>
       </c>
       <c r="B2" t="s">
-        <v>277</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -3141,16 +3183,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>371</v>
+        <v>385</v>
       </c>
       <c r="B1" t="s">
-        <v>372</v>
+        <v>386</v>
       </c>
       <c r="C1" t="s">
-        <v>374</v>
+        <v>388</v>
       </c>
       <c r="D1" t="s">
-        <v>376</v>
+        <v>390</v>
       </c>
     </row>
     <row r="2">
@@ -3158,13 +3200,13 @@
         <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>373</v>
+        <v>387</v>
       </c>
       <c r="C2" t="s">
-        <v>375</v>
+        <v>389</v>
       </c>
       <c r="D2" t="s">
-        <v>377</v>
+        <v>391</v>
       </c>
     </row>
   </sheetData>
@@ -3298,7 +3340,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3416,6 +3458,30 @@
         <v>124</v>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>125</v>
+      </c>
+      <c r="B15" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>127</v>
+      </c>
+      <c r="B16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>129</v>
+      </c>
+      <c r="B17" t="s">
+        <v>130</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -3423,7 +3489,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3431,306 +3497,338 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="B1" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B3" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="B4" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="B5" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="B6" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="B7" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="B8" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="B9" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="B10" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="B11" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="B12" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="B13" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="B14" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="B15" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="B16" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="B17" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="B18" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="B19" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="B20" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="B21" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="B22" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="B23" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="B24" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B25" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="B26" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="B27" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="B28" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="B29" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="B30" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="B31" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="B32" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="B33" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="B34" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="B35" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="B36" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="B37" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="B38" t="s">
-        <v>201</v>
+        <v>207</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>208</v>
+      </c>
+      <c r="B39" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>210</v>
+      </c>
+      <c r="B40" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>212</v>
+      </c>
+      <c r="B41" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>214</v>
+      </c>
+      <c r="B42" t="s">
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -3748,42 +3846,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>204</v>
+        <v>218</v>
       </c>
       <c r="B1" t="s">
-        <v>205</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>206</v>
+        <v>220</v>
       </c>
       <c r="B2" t="s">
-        <v>207</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>208</v>
+        <v>222</v>
       </c>
       <c r="B3" t="s">
-        <v>209</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>210</v>
+        <v>224</v>
       </c>
       <c r="B4" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="B5" t="s">
-        <v>213</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -3801,26 +3899,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>206</v>
+        <v>220</v>
       </c>
       <c r="B1" t="s">
-        <v>207</v>
+        <v>221</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>208</v>
+        <v>222</v>
       </c>
       <c r="B2" t="s">
-        <v>209</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>210</v>
+        <v>224</v>
       </c>
       <c r="B3" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -3838,32 +3936,32 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>219</v>
+        <v>233</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>220</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>221</v>
+        <v>235</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>222</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>223</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>224</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added microliter 'ul' option in 'library_input_amount_unit' and 'library_output_amount_unit' fields
</commit_message>
<xml_diff>
--- a/atacseq/latest/atacseq.xlsx
+++ b/atacseq/latest/atacseq.xlsx
@@ -381,7 +381,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="432">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -491,6 +491,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000300</t>
   </si>
   <si>
+    <t>MUSIC</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000328</t>
+  </si>
+  <si>
     <t>CyCIF</t>
   </si>
   <si>
@@ -596,6 +602,12 @@
     <t>analyte_class</t>
   </si>
   <si>
+    <t>DNA + RNA</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000327</t>
+  </si>
+  <si>
     <t>Chromatin</t>
   </si>
   <si>
@@ -770,6 +782,12 @@
     <t>https://identifiers.org/RRID:SCR_023609</t>
   </si>
   <si>
+    <t>Huron Digital Pathology</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024996</t>
+  </si>
+  <si>
     <t>Illumina</t>
   </si>
   <si>
@@ -839,6 +857,12 @@
     <t>https://identifiers.org/RRID:SCR_023616</t>
   </si>
   <si>
+    <t>PhenoImager Fusion</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023274</t>
+  </si>
+  <si>
     <t>DM6 B</t>
   </si>
   <si>
@@ -899,6 +923,12 @@
     <t>https://identifiers.org/RRID:SCR_023615</t>
   </si>
   <si>
+    <t>TissueScope LE Slide Scanner</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024995</t>
+  </si>
+  <si>
     <t>VS200 Slide Scanner</t>
   </si>
   <si>
@@ -983,6 +1013,12 @@
     <t>https://identifiers.org/RRID:SCR_023617</t>
   </si>
   <si>
+    <t>Aperio AT2</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_021256</t>
+  </si>
+  <si>
     <t>MIBIscope</t>
   </si>
   <si>
@@ -1238,6 +1274,12 @@
     <t>http://purl.obolibrary.org/obo/UO_0000024</t>
   </si>
   <si>
+    <t>ul</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000101</t>
+  </si>
+  <si>
     <t>library_output_amount_value</t>
   </si>
   <si>
@@ -1289,6 +1331,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000250</t>
   </si>
   <si>
+    <t>10X Genomics; Visium CytAssist Spatial Gene Expression for FFPE, Human Transcriptome, 11 mm, 2 reactions; PN 1000522</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000322</t>
+  </si>
+  <si>
     <t>10X Genomics; Visium Spatial Gene Expression Slide and Reagent Kit, 4 slides, 16 reactions; PN 1000184</t>
   </si>
   <si>
@@ -1307,6 +1355,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000260</t>
   </si>
   <si>
+    <t>10X Genomics; Visium Spatial for FFPE Gene Expression Kit, Human Transcriptome, 1 slides, 4 reactions; PN 1000338</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000320</t>
+  </si>
+  <si>
     <t>10X Genomics; Chromium Single Cell 3' Library &amp; Gel Bead Kit, 4 rxns; PN-120267</t>
   </si>
   <si>
@@ -1325,6 +1379,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000265</t>
   </si>
   <si>
+    <t>10X Genomics; Visium CytAssist Spatial Gene Expression for FFPE, Human Transcriptome, 6.5mm, 4 reactions; PN 1000520</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000321</t>
+  </si>
+  <si>
     <t>sample_indexing_kit</t>
   </si>
   <si>
@@ -1388,6 +1448,18 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000254</t>
   </si>
   <si>
+    <t>Illumina; NovaSeq 6000 S1 Reagent v1.5 Kit (300 Cycles); PN 20028317</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000318</t>
+  </si>
+  <si>
+    <t>Illumina; NextSeq 1000/2000 P2 Reagent v3 Kit (100 Cycles); PN 20046811</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000323</t>
+  </si>
+  <si>
     <t>Illumina; NovaSeq X Series 10B Reagent Kit (200 Cycle); PN 20085595</t>
   </si>
   <si>
@@ -1418,6 +1490,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000287</t>
   </si>
   <si>
+    <t>Illumina; NovaSeq 6000 S4 Reagent Kit v1.5 (300 cycles); PN 20028312</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000319</t>
+  </si>
+  <si>
     <t>Illumina; NovaSeq X Series 10B Reagent Kit (300 Cycle); PN 20085594</t>
   </si>
   <si>
@@ -1535,6 +1613,12 @@
     <t>https://identifiers.org/RRID:SCR_023731</t>
   </si>
   <si>
+    <t>ST5020 Multistainer</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_025021</t>
+  </si>
+  <si>
     <t>Chromium iX</t>
   </si>
   <si>
@@ -1556,6 +1640,18 @@
     <t>preparation_instrument_kit</t>
   </si>
   <si>
+    <t>10X Genomics; Visium FFPE Reagent Kit v2-Small, PN 1000436</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000324</t>
+  </si>
+  <si>
+    <t>10x Genomics; Chromium Next GEM Chip Q Single Cell Kit, 16 rxns; PN 1000422</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000325</t>
+  </si>
+  <si>
     <t>metadata_schema_id</t>
   </si>
   <si>
@@ -1574,7 +1670,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-01-29T14:34:33-08:00</t>
+    <t>2024-03-04T13:56:08-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1764,159 +1860,159 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>226</v>
+        <v>238</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>227</v>
+        <v>239</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>238</v>
+        <v>250</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>239</v>
+        <v>251</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>240</v>
+        <v>252</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>241</v>
+        <v>253</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>242</v>
+        <v>254</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>249</v>
+        <v>261</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>255</v>
+        <v>267</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>261</v>
+        <v>273</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>262</v>
+        <v>274</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>263</v>
+        <v>275</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>267</v>
+        <v>279</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>278</v>
+        <v>290</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>279</v>
+        <v>291</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>280</v>
+        <v>292</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>281</v>
+        <v>293</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>282</v>
+        <v>294</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>285</v>
+        <v>299</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>286</v>
+        <v>300</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>287</v>
+        <v>301</v>
       </c>
       <c r="AD1" t="s" s="1">
-        <v>288</v>
+        <v>302</v>
       </c>
       <c r="AE1" t="s" s="1">
-        <v>293</v>
+        <v>307</v>
       </c>
       <c r="AF1" t="s" s="1">
-        <v>298</v>
+        <v>312</v>
       </c>
       <c r="AG1" t="s" s="1">
-        <v>299</v>
+        <v>313</v>
       </c>
       <c r="AH1" t="s" s="1">
-        <v>314</v>
+        <v>334</v>
       </c>
       <c r="AI1" t="s" s="1">
-        <v>321</v>
+        <v>341</v>
       </c>
       <c r="AJ1" t="s" s="1">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="AK1" t="s" s="1">
-        <v>323</v>
+        <v>343</v>
       </c>
       <c r="AL1" t="s" s="1">
-        <v>324</v>
+        <v>344</v>
       </c>
       <c r="AM1" t="s" s="1">
-        <v>351</v>
+        <v>377</v>
       </c>
       <c r="AN1" t="s" s="1">
-        <v>352</v>
+        <v>378</v>
       </c>
       <c r="AO1" t="s" s="1">
-        <v>353</v>
+        <v>379</v>
       </c>
       <c r="AP1" t="s" s="1">
-        <v>360</v>
+        <v>386</v>
       </c>
       <c r="AQ1" t="s" s="1">
-        <v>361</v>
+        <v>387</v>
       </c>
       <c r="AR1" t="s" s="1">
-        <v>362</v>
+        <v>388</v>
       </c>
       <c r="AS1" t="s" s="1">
-        <v>369</v>
+        <v>395</v>
       </c>
       <c r="AT1" t="s" s="1">
-        <v>390</v>
+        <v>418</v>
       </c>
       <c r="AU1" t="s" s="1">
-        <v>391</v>
+        <v>423</v>
       </c>
     </row>
     <row r="2">
       <c r="D2" t="s" s="5">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="AU2" t="s" s="48">
-        <v>392</v>
+        <v>424</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="36">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$33</formula1>
+      <formula1>'dataset_type'!$A$1:$A$34</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'analyte_class'!$A$1:$A$11</formula1>
+      <formula1>'analyte_class'!$A$1:$A$12</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="F2:F1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'is_targeted'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_vendor'!$A$1:$A$19</formula1>
+      <formula1>'acquisition_instrument_vendor'!$A$1:$A$20</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$45</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$48</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -1966,14 +2062,14 @@
       <formula2>3.4028235E38</formula2>
     </dataValidation>
     <dataValidation type="list" sqref="Z2:Z1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'library_input_amount_unit'!$A$1:$A$1</formula1>
+      <formula1>'library_input_amount_unit'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="between" sqref="AA2:AA1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be a number" showErrorMessage="true">
       <formula1>-3.4028235E38</formula1>
       <formula2>3.4028235E38</formula2>
     </dataValidation>
     <dataValidation type="list" sqref="AB2:AB1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'library_output_amount_unit'!$A$1:$A$1</formula1>
+      <formula1>'library_output_amount_unit'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="between" sqref="AC2:AC1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be a number" showErrorMessage="true">
       <formula1>-3.4028235E38</formula1>
@@ -1990,7 +2086,7 @@
       <formula2>2147483647</formula2>
     </dataValidation>
     <dataValidation type="list" sqref="AG2:AG1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'library_preparation_kit'!$A$1:$A$7</formula1>
+      <formula1>'library_preparation_kit'!$A$1:$A$10</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AH2:AH1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'sample_indexing_kit'!$A$1:$A$4</formula1>
@@ -2003,7 +2099,7 @@
       <formula2>2147483647</formula2>
     </dataValidation>
     <dataValidation type="list" sqref="AL2:AL1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'sequencing_reagent_kit'!$A$1:$A$13</formula1>
+      <formula1>'sequencing_reagent_kit'!$A$1:$A$16</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AN2:AN1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'transposition_reagent_kit'!$A$1:$A$3</formula1>
@@ -2015,10 +2111,10 @@
       <formula1>'preparation_instrument_vendor'!$A$1:$A$7</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AS2:AS1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'preparation_instrument_model'!$A$1:$A$14</formula1>
+      <formula1>'preparation_instrument_model'!$A$1:$A$15</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AT2:AT1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'preparation_instrument_kit'!$A$1:$A$2</formula1>
+      <formula1>'preparation_instrument_kit'!$A$1:$A$4</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -2037,26 +2133,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>250</v>
+        <v>262</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>251</v>
+        <v>263</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>245</v>
+        <v>257</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>252</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>253</v>
+        <v>265</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>254</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -2074,32 +2170,32 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>256</v>
+        <v>268</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>257</v>
+        <v>269</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>245</v>
+        <v>257</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>258</v>
+        <v>270</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>259</v>
+        <v>271</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>260</v>
+        <v>272</v>
       </c>
     </row>
   </sheetData>
@@ -2117,17 +2213,17 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>243</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>245</v>
+        <v>257</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>258</v>
+        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -2145,26 +2241,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>250</v>
+        <v>262</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>251</v>
+        <v>263</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>245</v>
+        <v>257</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>252</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>253</v>
+        <v>265</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>254</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -2182,27 +2278,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>264</v>
+        <v>276</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>245</v>
+        <v>257</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>247</v>
+        <v>259</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>265</v>
+        <v>277</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>266</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -2220,42 +2316,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>268</v>
+        <v>280</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>269</v>
+        <v>281</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>270</v>
+        <v>282</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>271</v>
+        <v>283</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>272</v>
+        <v>284</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>273</v>
+        <v>285</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>274</v>
+        <v>286</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>275</v>
+        <v>287</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>276</v>
+        <v>288</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>277</v>
+        <v>289</v>
       </c>
     </row>
   </sheetData>
@@ -2265,7 +2361,7 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2273,10 +2369,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>283</v>
+        <v>295</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>284</v>
+        <v>296</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>297</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>298</v>
       </c>
     </row>
   </sheetData>
@@ -2286,7 +2390,7 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2294,10 +2398,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>283</v>
+        <v>295</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>284</v>
+        <v>296</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>297</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>298</v>
       </c>
     </row>
   </sheetData>
@@ -2315,18 +2427,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>289</v>
+        <v>303</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>290</v>
+        <v>304</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>291</v>
+        <v>305</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>292</v>
+        <v>306</v>
       </c>
     </row>
   </sheetData>
@@ -2344,18 +2456,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>294</v>
+        <v>308</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>295</v>
+        <v>309</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>296</v>
+        <v>310</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>297</v>
+        <v>311</v>
       </c>
     </row>
   </sheetData>
@@ -2365,7 +2477,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2635,6 +2747,14 @@
         <v>69</v>
       </c>
     </row>
+    <row r="34">
+      <c r="A34" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="B34" t="s" s="0">
+        <v>71</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -2642,7 +2762,7 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2650,58 +2770,82 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>300</v>
+        <v>314</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>301</v>
+        <v>315</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>302</v>
+        <v>316</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>303</v>
+        <v>317</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>304</v>
+        <v>318</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>305</v>
+        <v>319</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>306</v>
+        <v>320</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>307</v>
+        <v>321</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>308</v>
+        <v>322</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>309</v>
+        <v>323</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>310</v>
+        <v>324</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>311</v>
+        <v>325</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>313</v>
+        <v>327</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>328</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>330</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>332</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>333</v>
       </c>
     </row>
   </sheetData>
@@ -2719,34 +2863,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>315</v>
+        <v>335</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>316</v>
+        <v>336</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>245</v>
+        <v>257</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>252</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>317</v>
+        <v>337</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>318</v>
+        <v>338</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>319</v>
+        <v>339</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>320</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>
@@ -2764,12 +2908,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -2779,7 +2923,7 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2787,106 +2931,130 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>325</v>
+        <v>345</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>326</v>
+        <v>346</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>327</v>
+        <v>347</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>328</v>
+        <v>348</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>329</v>
+        <v>349</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>330</v>
+        <v>350</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>331</v>
+        <v>351</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>332</v>
+        <v>352</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>333</v>
+        <v>353</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>334</v>
+        <v>354</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>335</v>
+        <v>355</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>336</v>
+        <v>356</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>337</v>
+        <v>357</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>338</v>
+        <v>358</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>339</v>
+        <v>359</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>340</v>
+        <v>360</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>341</v>
+        <v>361</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>342</v>
+        <v>362</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>343</v>
+        <v>363</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>344</v>
+        <v>364</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>345</v>
+        <v>365</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>346</v>
+        <v>366</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>347</v>
+        <v>367</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>348</v>
+        <v>368</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>349</v>
+        <v>369</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>350</v>
+        <v>370</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="0">
+        <v>371</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>373</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="0">
+        <v>375</v>
+      </c>
+      <c r="B16" t="s" s="0">
+        <v>376</v>
       </c>
     </row>
   </sheetData>
@@ -2904,26 +3072,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>304</v>
+        <v>320</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>305</v>
+        <v>321</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>300</v>
+        <v>314</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>301</v>
+        <v>315</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>245</v>
+        <v>257</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>252</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -2941,26 +3109,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>354</v>
+        <v>380</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>355</v>
+        <v>381</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>356</v>
+        <v>382</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>357</v>
+        <v>383</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>358</v>
+        <v>384</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>359</v>
+        <v>385</v>
       </c>
     </row>
   </sheetData>
@@ -2978,58 +3146,58 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>245</v>
+        <v>257</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>252</v>
+        <v>264</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>363</v>
+        <v>389</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>364</v>
+        <v>390</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>365</v>
+        <v>391</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>366</v>
+        <v>392</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>367</v>
+        <v>393</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>368</v>
+        <v>394</v>
       </c>
     </row>
   </sheetData>
@@ -3039,7 +3207,7 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3047,114 +3215,122 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>143</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>245</v>
+        <v>257</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>252</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>370</v>
+        <v>396</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>371</v>
+        <v>397</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>372</v>
+        <v>398</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>373</v>
+        <v>399</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>204</v>
+        <v>216</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>205</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>207</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>374</v>
+        <v>400</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>375</v>
+        <v>401</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>376</v>
+        <v>402</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>377</v>
+        <v>403</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>378</v>
+        <v>404</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>379</v>
+        <v>405</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>380</v>
+        <v>406</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>381</v>
+        <v>407</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>382</v>
+        <v>408</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>383</v>
+        <v>409</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>384</v>
+        <v>410</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>385</v>
+        <v>411</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>386</v>
+        <v>412</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>387</v>
+        <v>413</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>388</v>
+        <v>414</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>389</v>
+        <v>415</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>416</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>417</v>
       </c>
     </row>
   </sheetData>
@@ -3164,7 +3340,7 @@
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3172,18 +3348,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>304</v>
+        <v>320</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>305</v>
+        <v>321</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>300</v>
+        <v>314</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>301</v>
+        <v>315</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>419</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>421</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>422</v>
       </c>
     </row>
   </sheetData>
@@ -3207,30 +3399,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>393</v>
+        <v>425</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>394</v>
+        <v>426</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>396</v>
+        <v>428</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>398</v>
+        <v>430</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>395</v>
+        <v>427</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>397</v>
+        <v>429</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>399</v>
+        <v>431</v>
       </c>
     </row>
   </sheetData>
@@ -3240,7 +3432,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3248,90 +3440,98 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>92</v>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -3349,12 +3549,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -3364,7 +3564,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3372,154 +3572,162 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>134</v>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>139</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -3529,7 +3737,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:B48"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3537,362 +3745,386 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>137</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>139</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>141</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>143</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>145</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>147</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>149</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>151</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>153</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>157</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>161</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>163</v>
+        <v>169</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>165</v>
+        <v>171</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>167</v>
+        <v>173</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>169</v>
+        <v>175</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>173</v>
+        <v>179</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>175</v>
+        <v>181</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>177</v>
+        <v>183</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>179</v>
+        <v>185</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>181</v>
+        <v>187</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>185</v>
+        <v>191</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>187</v>
+        <v>193</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>189</v>
+        <v>195</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>191</v>
+        <v>197</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>193</v>
+        <v>199</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>195</v>
+        <v>201</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>197</v>
+        <v>203</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>199</v>
+        <v>205</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>203</v>
+        <v>209</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>205</v>
+        <v>211</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>207</v>
+        <v>213</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>209</v>
+        <v>215</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>211</v>
+        <v>217</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>213</v>
+        <v>219</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>217</v>
+        <v>223</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>219</v>
+        <v>225</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>221</v>
+        <v>227</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>223</v>
+        <v>229</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>225</v>
+        <v>231</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>232</v>
+      </c>
+      <c r="B46" t="s" s="0">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
+        <v>234</v>
+      </c>
+      <c r="B47" t="s" s="0">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="0">
+        <v>236</v>
+      </c>
+      <c r="B48" t="s" s="0">
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -3910,42 +4142,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>228</v>
+        <v>240</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>229</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>230</v>
+        <v>242</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>231</v>
+        <v>243</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>233</v>
+        <v>245</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>234</v>
+        <v>246</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>235</v>
+        <v>247</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>236</v>
+        <v>248</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>237</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -3963,26 +4195,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>230</v>
+        <v>242</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>231</v>
+        <v>243</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>233</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>234</v>
+        <v>246</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>235</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -4000,32 +4232,32 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>243</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>244</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>245</v>
+        <v>257</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>246</v>
+        <v>258</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>247</v>
+        <v>259</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>248</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added "20" in barcode_offset and "36" in umi_offset
Closes #8
</commit_message>
<xml_diff>
--- a/atacseq/latest/atacseq.xlsx
+++ b/atacseq/latest/atacseq.xlsx
@@ -381,7 +381,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="436">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -827,30 +827,144 @@
     <t>https://identifiers.org/RRID:SCR_017202</t>
   </si>
   <si>
+    <t>MoticEasyScan One</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024855</t>
+  </si>
+  <si>
+    <t>EVOS M7000</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_025070</t>
+  </si>
+  <si>
+    <t>NovaSeq X</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024569</t>
+  </si>
+  <si>
+    <t>NanoZoomer 2.0-HT</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_021658</t>
+  </si>
+  <si>
+    <t>Lightsheet 7</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024448</t>
+  </si>
+  <si>
+    <t>Phenocycler-Fusion 1.0</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000316</t>
+  </si>
+  <si>
+    <t>DNBSEQ-T7</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024847</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C17998</t>
+  </si>
+  <si>
+    <t>Q Exactive UHMR</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_020571</t>
+  </si>
+  <si>
+    <t>Q Exactive</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_020565</t>
+  </si>
+  <si>
+    <t>Zyla 4.2 sCMOS</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023610</t>
+  </si>
+  <si>
+    <t>Custom: Multiphoton</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000317</t>
+  </si>
+  <si>
+    <t>QTRAP 5500</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_020517</t>
+  </si>
+  <si>
+    <t>BZ-X800</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023617</t>
+  </si>
+  <si>
+    <t>NextSeq 500</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_014983</t>
+  </si>
+  <si>
+    <t>NanoZoomer S360</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023761</t>
+  </si>
+  <si>
+    <t>Hyperion Imaging System</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023195</t>
+  </si>
+  <si>
+    <t>NovaSeq X Plus</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024568</t>
+  </si>
+  <si>
+    <t>NanoZoomer-SQ</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023763</t>
+  </si>
+  <si>
+    <t>NextSeq 550</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_016381</t>
+  </si>
+  <si>
+    <t>Digital Spatial Profiler</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_021660</t>
+  </si>
+  <si>
     <t>NanoZoomer S210</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_023760</t>
   </si>
   <si>
-    <t>MoticEasyScan One</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024855</t>
-  </si>
-  <si>
     <t>Axio Observer 7</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_023694</t>
   </si>
   <si>
-    <t>NovaSeq X</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024569</t>
-  </si>
-  <si>
     <t>IN Cell Analyzer 2200</t>
   </si>
   <si>
@@ -869,36 +983,12 @@
     <t>https://identifiers.org/RRID:SCR_024857</t>
   </si>
   <si>
-    <t>NanoZoomer 2.0-HT</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_021658</t>
-  </si>
-  <si>
     <t>Phenocycler-Fusion 2.0</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_023773</t>
   </si>
   <si>
-    <t>Lightsheet 7</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024448</t>
-  </si>
-  <si>
-    <t>Phenocycler-Fusion 1.0</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000316</t>
-  </si>
-  <si>
-    <t>DNBSEQ-T7</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024847</t>
-  </si>
-  <si>
     <t>Orbitrap Fusion Lumos Tribrid</t>
   </si>
   <si>
@@ -911,12 +1001,6 @@
     <t>https://identifiers.org/RRID:SCR_024449</t>
   </si>
   <si>
-    <t>Unknown</t>
-  </si>
-  <si>
-    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C17998</t>
-  </si>
-  <si>
     <t>MALDI timsTOF Flex Prototype</t>
   </si>
   <si>
@@ -959,12 +1043,6 @@
     <t>https://identifiers.org/RRID:SCR_023618</t>
   </si>
   <si>
-    <t>Q Exactive UHMR</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_020571</t>
-  </si>
-  <si>
     <t>NextSeq 2000</t>
   </si>
   <si>
@@ -977,42 +1055,12 @@
     <t>https://identifiers.org/RRID:SCR_016387</t>
   </si>
   <si>
-    <t>Q Exactive</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_020565</t>
-  </si>
-  <si>
-    <t>Zyla 4.2 sCMOS</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023610</t>
-  </si>
-  <si>
     <t>HiSeq 4000</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_016386</t>
   </si>
   <si>
-    <t>Custom: Multiphoton</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000317</t>
-  </si>
-  <si>
-    <t>QTRAP 5500</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_020517</t>
-  </si>
-  <si>
-    <t>BZ-X800</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023617</t>
-  </si>
-  <si>
     <t>Aperio AT2</t>
   </si>
   <si>
@@ -1025,18 +1073,6 @@
     <t>https://identifiers.org/RRID:SCR_023613</t>
   </si>
   <si>
-    <t>NextSeq 500</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_014983</t>
-  </si>
-  <si>
-    <t>NanoZoomer S360</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023761</t>
-  </si>
-  <si>
     <t>NanoZoomer S60</t>
   </si>
   <si>
@@ -1049,36 +1085,6 @@
     <t>https://identifiers.org/RRID:SCR_023909</t>
   </si>
   <si>
-    <t>Hyperion Imaging System</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023195</t>
-  </si>
-  <si>
-    <t>NovaSeq X Plus</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024568</t>
-  </si>
-  <si>
-    <t>NanoZoomer-SQ</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023763</t>
-  </si>
-  <si>
-    <t>NextSeq 550</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_016381</t>
-  </si>
-  <si>
-    <t>Digital Spatial Profiler</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_021660</t>
-  </si>
-  <si>
     <t>Axio Scan.Z1</t>
   </si>
   <si>
@@ -1166,6 +1172,9 @@
     <t>10,48,86</t>
   </si>
   <si>
+    <t>20</t>
+  </si>
+  <si>
     <t>barcode_read</t>
   </si>
   <si>
@@ -1205,6 +1214,9 @@
     <t>umi_offset</t>
   </si>
   <si>
+    <t>36</t>
+  </si>
+  <si>
     <t>umi_read</t>
   </si>
   <si>
@@ -1670,7 +1682,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-03-04T13:56:08-08:00</t>
+    <t>2024-03-05T18:56:30-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1872,121 +1884,121 @@
         <v>141</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="AD1" t="s" s="1">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="AE1" t="s" s="1">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="AF1" t="s" s="1">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="AG1" t="s" s="1">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="AH1" t="s" s="1">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="AI1" t="s" s="1">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="AJ1" t="s" s="1">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="AK1" t="s" s="1">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="AL1" t="s" s="1">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="AM1" t="s" s="1">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="AN1" t="s" s="1">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="AO1" t="s" s="1">
-        <v>379</v>
+        <v>383</v>
       </c>
       <c r="AP1" t="s" s="1">
-        <v>386</v>
+        <v>390</v>
       </c>
       <c r="AQ1" t="s" s="1">
-        <v>387</v>
+        <v>391</v>
       </c>
       <c r="AR1" t="s" s="1">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="AS1" t="s" s="1">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="AT1" t="s" s="1">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="AU1" t="s" s="1">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="2">
@@ -1994,7 +2006,7 @@
         <v>46</v>
       </c>
       <c r="AU2" t="s" s="48">
-        <v>424</v>
+        <v>428</v>
       </c>
     </row>
   </sheetData>
@@ -2012,7 +2024,7 @@
       <formula1>'acquisition_instrument_vendor'!$A$1:$A$20</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$48</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$49</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -2029,7 +2041,7 @@
       <formula1>'time_since_acquisition_instrume'!$A$1:$A$3</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="O2:O1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'barcode_offset'!$A$1:$A$6</formula1>
+      <formula1>'barcode_offset'!$A$1:$A$7</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="P2:P1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'barcode_read'!$A$1:$A$3</formula1>
@@ -2038,7 +2050,7 @@
       <formula1>'barcode_size'!$A$1:$A$6</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="R2:R1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'umi_offset'!$A$1:$A$3</formula1>
+      <formula1>'umi_offset'!$A$1:$A$4</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="S2:S1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'umi_read'!$A$1:$A$3</formula1>
@@ -2133,26 +2145,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>266</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -2170,32 +2182,32 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>269</v>
+        <v>272</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>270</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>272</v>
+        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -2205,7 +2217,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2213,17 +2225,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>257</v>
+        <v>277</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>270</v>
+        <v>259</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -2241,26 +2258,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>266</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -2278,27 +2295,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>276</v>
+        <v>280</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>278</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -2316,42 +2333,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>281</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>283</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>285</v>
+        <v>289</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>287</v>
+        <v>291</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>289</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>
@@ -2369,18 +2386,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>296</v>
+        <v>300</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>298</v>
+        <v>302</v>
       </c>
     </row>
   </sheetData>
@@ -2398,18 +2415,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>296</v>
+        <v>300</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>298</v>
+        <v>302</v>
       </c>
     </row>
   </sheetData>
@@ -2427,18 +2444,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>304</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>306</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>
@@ -2456,18 +2473,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>309</v>
+        <v>313</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>311</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>
@@ -2770,82 +2787,82 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>315</v>
+        <v>319</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>317</v>
+        <v>321</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>319</v>
+        <v>323</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>321</v>
+        <v>325</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>323</v>
+        <v>327</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>325</v>
+        <v>329</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>327</v>
+        <v>331</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>329</v>
+        <v>333</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>331</v>
+        <v>335</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>333</v>
+        <v>337</v>
       </c>
     </row>
   </sheetData>
@@ -2863,34 +2880,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>336</v>
+        <v>340</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>338</v>
+        <v>342</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>340</v>
+        <v>344</v>
       </c>
     </row>
   </sheetData>
@@ -2931,130 +2948,130 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>346</v>
+        <v>350</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>348</v>
+        <v>352</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>350</v>
+        <v>354</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>352</v>
+        <v>356</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>354</v>
+        <v>358</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>356</v>
+        <v>360</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>358</v>
+        <v>362</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>360</v>
+        <v>364</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>362</v>
+        <v>366</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>364</v>
+        <v>368</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>366</v>
+        <v>370</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>368</v>
+        <v>372</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>370</v>
+        <v>374</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>371</v>
+        <v>375</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>372</v>
+        <v>376</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>374</v>
+        <v>378</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>376</v>
+        <v>380</v>
       </c>
     </row>
   </sheetData>
@@ -3072,26 +3089,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>321</v>
+        <v>325</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>315</v>
+        <v>319</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -3109,26 +3126,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>381</v>
+        <v>385</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>382</v>
+        <v>386</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>383</v>
+        <v>387</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>385</v>
+        <v>389</v>
       </c>
     </row>
   </sheetData>
@@ -3162,26 +3179,26 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>390</v>
+        <v>394</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>392</v>
+        <v>396</v>
       </c>
     </row>
     <row r="6">
@@ -3194,10 +3211,10 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>394</v>
+        <v>398</v>
       </c>
     </row>
   </sheetData>
@@ -3215,122 +3232,122 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>148</v>
+        <v>190</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>149</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>397</v>
+        <v>401</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>398</v>
+        <v>402</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>399</v>
+        <v>403</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>216</v>
+        <v>178</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>217</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>218</v>
+        <v>230</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>219</v>
+        <v>231</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>401</v>
+        <v>405</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>403</v>
+        <v>407</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>404</v>
+        <v>408</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>405</v>
+        <v>409</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>407</v>
+        <v>411</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>409</v>
+        <v>413</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>411</v>
+        <v>415</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>413</v>
+        <v>417</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>414</v>
+        <v>418</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>415</v>
+        <v>419</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>417</v>
+        <v>421</v>
       </c>
     </row>
   </sheetData>
@@ -3348,34 +3365,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>321</v>
+        <v>325</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>315</v>
+        <v>319</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>420</v>
+        <v>424</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>422</v>
+        <v>426</v>
       </c>
     </row>
   </sheetData>
@@ -3399,16 +3416,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>425</v>
+        <v>429</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>426</v>
+        <v>430</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>430</v>
+        <v>434</v>
       </c>
     </row>
     <row r="2">
@@ -3416,13 +3433,13 @@
         <v>46</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>431</v>
+        <v>435</v>
       </c>
     </row>
   </sheetData>
@@ -3737,7 +3754,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4125,6 +4142,14 @@
       </c>
       <c r="B48" t="s" s="0">
         <v>237</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="0">
+        <v>238</v>
+      </c>
+      <c r="B49" t="s" s="0">
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -4142,42 +4167,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -4195,26 +4220,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -4224,7 +4249,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4232,32 +4257,37 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>260</v>
+        <v>262</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the missing library preparation kit
Closes #93
</commit_message>
<xml_diff>
--- a/atacseq/latest/atacseq.xlsx
+++ b/atacseq/latest/atacseq.xlsx
@@ -6,7 +6,7 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="ATACseq v3" r:id="rId3" sheetId="1"/>
+    <sheet name="ATACseq" r:id="rId3" sheetId="1"/>
     <sheet name="dataset_type" r:id="rId4" sheetId="2"/>
     <sheet name="analyte_class" r:id="rId5" sheetId="3"/>
     <sheet name="is_targeted" r:id="rId6" sheetId="4"/>
@@ -381,7 +381,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="616">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -539,6 +539,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000309</t>
   </si>
   <si>
+    <t>CosMx Proteomics</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000435</t>
+  </si>
+  <si>
     <t>Histology</t>
   </si>
   <si>
@@ -776,6 +782,18 @@
     <t>https://identifiers.org/RRID:SCR_023607</t>
   </si>
   <si>
+    <t>Complete Genomics</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027007</t>
+  </si>
+  <si>
+    <t>3DHISTECH</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027042</t>
+  </si>
+  <si>
     <t>GE Healthcare</t>
   </si>
   <si>
@@ -929,6 +947,12 @@
     <t>https://identifiers.org/RRID:SCR_017202</t>
   </si>
   <si>
+    <t>Pannoramic MIDI II Digital Scanner</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024834</t>
+  </si>
+  <si>
     <t>Not applicable</t>
   </si>
   <si>
@@ -1514,6 +1538,12 @@
     <t>http://purl.obolibrary.org/obo/UO_0010050</t>
   </si>
   <si>
+    <t>pg/ul</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000438</t>
+  </si>
+  <si>
     <t>nM</t>
   </si>
   <si>
@@ -1655,6 +1685,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000394</t>
   </si>
   <si>
+    <t>10x Genomics; Library Construction Kit, 16 rxns; PN 1000190</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000439</t>
+  </si>
+  <si>
     <t>Parse Biosciences; Evercode WT Mini v2 Kit, 12 rxns; PN ECW02010</t>
   </si>
   <si>
@@ -2177,9 +2213,6 @@
     <t>schema:title</t>
   </si>
   <si>
-    <t>ATACseq v3</t>
-  </si>
-  <si>
     <t>pav:version</t>
   </si>
   <si>
@@ -2189,7 +2222,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-05-12T10:14:57-07:00</t>
+    <t>2025-06-10T14:22:23-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -2379,133 +2412,133 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>310</v>
+        <v>318</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>311</v>
+        <v>319</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>322</v>
+        <v>330</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>323</v>
+        <v>331</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>324</v>
+        <v>332</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>325</v>
+        <v>333</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>333</v>
+        <v>341</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>338</v>
+        <v>346</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>344</v>
+        <v>352</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>346</v>
+        <v>354</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>347</v>
+        <v>355</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>351</v>
+        <v>359</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>362</v>
+        <v>370</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>363</v>
+        <v>371</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>364</v>
+        <v>372</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>365</v>
+        <v>373</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>366</v>
+        <v>374</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>371</v>
+        <v>379</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>372</v>
+        <v>380</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>373</v>
+        <v>381</v>
       </c>
       <c r="AD1" t="s" s="1">
-        <v>374</v>
+        <v>382</v>
       </c>
       <c r="AE1" t="s" s="1">
-        <v>379</v>
+        <v>389</v>
       </c>
       <c r="AF1" t="s" s="1">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="AG1" t="s" s="1">
-        <v>385</v>
+        <v>395</v>
       </c>
       <c r="AH1" t="s" s="1">
-        <v>448</v>
+        <v>460</v>
       </c>
       <c r="AI1" t="s" s="1">
-        <v>479</v>
+        <v>491</v>
       </c>
       <c r="AJ1" t="s" s="1">
-        <v>480</v>
+        <v>492</v>
       </c>
       <c r="AK1" t="s" s="1">
-        <v>481</v>
+        <v>493</v>
       </c>
       <c r="AL1" t="s" s="1">
-        <v>482</v>
+        <v>494</v>
       </c>
       <c r="AM1" t="s" s="1">
-        <v>533</v>
+        <v>545</v>
       </c>
       <c r="AN1" t="s" s="1">
-        <v>534</v>
+        <v>546</v>
       </c>
       <c r="AO1" t="s" s="1">
-        <v>535</v>
+        <v>547</v>
       </c>
       <c r="AP1" t="s" s="1">
-        <v>542</v>
+        <v>554</v>
       </c>
       <c r="AQ1" t="s" s="1">
-        <v>543</v>
+        <v>555</v>
       </c>
       <c r="AR1" t="s" s="1">
-        <v>544</v>
+        <v>556</v>
       </c>
       <c r="AS1" t="s" s="1">
-        <v>551</v>
+        <v>563</v>
       </c>
       <c r="AT1" t="s" s="1">
-        <v>578</v>
+        <v>590</v>
       </c>
       <c r="AU1" t="s" s="1">
-        <v>595</v>
+        <v>607</v>
       </c>
     </row>
     <row r="2">
@@ -2513,13 +2546,13 @@
         <v>50</v>
       </c>
       <c r="AU2" t="s" s="48">
-        <v>596</v>
+        <v>608</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="36">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$41</formula1>
+      <formula1>'dataset_type'!$A$1:$A$42</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'analyte_class'!$A$1:$A$16</formula1>
@@ -2528,10 +2561,10 @@
       <formula1>'is_targeted'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_vendor'!$A$1:$A$26</formula1>
+      <formula1>'acquisition_instrument_vendor'!$A$1:$A$28</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$68</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$69</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -2595,7 +2628,7 @@
       <formula2>3.4028235E38</formula2>
     </dataValidation>
     <dataValidation type="list" sqref="AD2:AD1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'library_concentration_unit'!$A$1:$A$2</formula1>
+      <formula1>'library_concentration_unit'!$A$1:$A$3</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AE2:AE1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'library_layout'!$A$1:$A$2</formula1>
@@ -2605,7 +2638,7 @@
       <formula2>2147483647</formula2>
     </dataValidation>
     <dataValidation type="list" sqref="AG2:AG1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'library_preparation_kit'!$A$1:$A$31</formula1>
+      <formula1>'library_preparation_kit'!$A$1:$A$32</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AH2:AH1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'sample_indexing_kit'!$A$1:$A$17</formula1>
@@ -2652,26 +2685,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>334</v>
+        <v>342</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>335</v>
+        <v>343</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>183</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>336</v>
+        <v>344</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>337</v>
+        <v>345</v>
       </c>
     </row>
   </sheetData>
@@ -2689,32 +2722,32 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>339</v>
+        <v>347</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>340</v>
+        <v>348</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>341</v>
+        <v>349</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>342</v>
+        <v>350</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>343</v>
+        <v>351</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>182</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -2732,22 +2765,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>327</v>
+        <v>335</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>340</v>
+        <v>348</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>345</v>
+        <v>353</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>182</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -2765,26 +2798,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>334</v>
+        <v>342</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>335</v>
+        <v>343</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>183</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>336</v>
+        <v>344</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>337</v>
+        <v>345</v>
       </c>
     </row>
   </sheetData>
@@ -2802,27 +2835,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>328</v>
+        <v>336</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>348</v>
+        <v>356</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>349</v>
+        <v>357</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>350</v>
+        <v>358</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>182</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -2840,42 +2873,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>352</v>
+        <v>360</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>353</v>
+        <v>361</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>354</v>
+        <v>362</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>355</v>
+        <v>363</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>356</v>
+        <v>364</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>357</v>
+        <v>365</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>358</v>
+        <v>366</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>359</v>
+        <v>367</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>360</v>
+        <v>368</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>361</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -2893,18 +2926,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>367</v>
+        <v>375</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>368</v>
+        <v>376</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>369</v>
+        <v>377</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>370</v>
+        <v>378</v>
       </c>
     </row>
   </sheetData>
@@ -2922,18 +2955,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>367</v>
+        <v>375</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>368</v>
+        <v>376</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>369</v>
+        <v>377</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>370</v>
+        <v>378</v>
       </c>
     </row>
   </sheetData>
@@ -2943,7 +2976,7 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2951,18 +2984,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>375</v>
+        <v>383</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>376</v>
+        <v>384</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>377</v>
+        <v>385</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>378</v>
+        <v>386</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>387</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>388</v>
       </c>
     </row>
   </sheetData>
@@ -2980,18 +3021,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>380</v>
+        <v>390</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>381</v>
+        <v>391</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>382</v>
+        <v>392</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>383</v>
+        <v>393</v>
       </c>
     </row>
   </sheetData>
@@ -3001,7 +3042,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3335,6 +3376,14 @@
         <v>85</v>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" t="s" s="0">
+        <v>86</v>
+      </c>
+      <c r="B42" t="s" s="0">
+        <v>87</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -3342,7 +3391,7 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3350,250 +3399,258 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>386</v>
+        <v>396</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>387</v>
+        <v>397</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>388</v>
+        <v>398</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>389</v>
+        <v>399</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>391</v>
+        <v>401</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>392</v>
+        <v>402</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>393</v>
+        <v>403</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>394</v>
+        <v>404</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>395</v>
+        <v>405</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>396</v>
+        <v>406</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>397</v>
+        <v>407</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>398</v>
+        <v>408</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>399</v>
+        <v>409</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>400</v>
+        <v>410</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>401</v>
+        <v>411</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>402</v>
+        <v>412</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>403</v>
+        <v>413</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>404</v>
+        <v>414</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>405</v>
+        <v>415</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>406</v>
+        <v>416</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>407</v>
+        <v>417</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>408</v>
+        <v>418</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>409</v>
+        <v>419</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>410</v>
+        <v>420</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>411</v>
+        <v>421</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>412</v>
+        <v>422</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>413</v>
+        <v>423</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>414</v>
+        <v>424</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>415</v>
+        <v>425</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>416</v>
+        <v>426</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>417</v>
+        <v>427</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>418</v>
+        <v>428</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>419</v>
+        <v>429</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>420</v>
+        <v>430</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>421</v>
+        <v>431</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>422</v>
+        <v>432</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>423</v>
+        <v>433</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>424</v>
+        <v>434</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>425</v>
+        <v>435</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>426</v>
+        <v>436</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>427</v>
+        <v>437</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>428</v>
+        <v>438</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>429</v>
+        <v>439</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>430</v>
+        <v>440</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>431</v>
+        <v>441</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>432</v>
+        <v>442</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>433</v>
+        <v>443</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>434</v>
+        <v>444</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>435</v>
+        <v>445</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>436</v>
+        <v>446</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>437</v>
+        <v>447</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>438</v>
+        <v>448</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>439</v>
+        <v>449</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>440</v>
+        <v>450</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>441</v>
+        <v>451</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>442</v>
+        <v>452</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>443</v>
+        <v>453</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>444</v>
+        <v>454</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>445</v>
+        <v>455</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>446</v>
+        <v>456</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>447</v>
+        <v>457</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="0">
+        <v>458</v>
+      </c>
+      <c r="B32" t="s" s="0">
+        <v>459</v>
       </c>
     </row>
   </sheetData>
@@ -3611,138 +3668,138 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>449</v>
+        <v>461</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>450</v>
+        <v>462</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>183</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>451</v>
+        <v>463</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>452</v>
+        <v>464</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>453</v>
+        <v>465</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>454</v>
+        <v>466</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>455</v>
+        <v>467</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>456</v>
+        <v>468</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>457</v>
+        <v>469</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>458</v>
+        <v>470</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>460</v>
+        <v>472</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>461</v>
+        <v>473</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>462</v>
+        <v>474</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>463</v>
+        <v>475</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>464</v>
+        <v>476</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>434</v>
+        <v>446</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>435</v>
+        <v>447</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>465</v>
+        <v>477</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>466</v>
+        <v>478</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>467</v>
+        <v>479</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>468</v>
+        <v>480</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>469</v>
+        <v>481</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>470</v>
+        <v>482</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>471</v>
+        <v>483</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>472</v>
+        <v>484</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>473</v>
+        <v>485</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>474</v>
+        <v>486</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>475</v>
+        <v>487</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>476</v>
+        <v>488</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>477</v>
+        <v>489</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>478</v>
+        <v>490</v>
       </c>
     </row>
   </sheetData>
@@ -3760,12 +3817,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -3783,210 +3840,210 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>483</v>
+        <v>495</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>484</v>
+        <v>496</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>485</v>
+        <v>497</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>486</v>
+        <v>498</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>487</v>
+        <v>499</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>488</v>
+        <v>500</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>489</v>
+        <v>501</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>490</v>
+        <v>502</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>491</v>
+        <v>503</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>492</v>
+        <v>504</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>493</v>
+        <v>505</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>494</v>
+        <v>506</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>495</v>
+        <v>507</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>496</v>
+        <v>508</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>497</v>
+        <v>509</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>498</v>
+        <v>510</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>499</v>
+        <v>511</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>500</v>
+        <v>512</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>501</v>
+        <v>513</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>502</v>
+        <v>514</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>503</v>
+        <v>515</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>504</v>
+        <v>516</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>505</v>
+        <v>517</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>506</v>
+        <v>518</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>507</v>
+        <v>519</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>508</v>
+        <v>520</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>509</v>
+        <v>521</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>510</v>
+        <v>522</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>511</v>
+        <v>523</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>512</v>
+        <v>524</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>434</v>
+        <v>446</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>435</v>
+        <v>447</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>513</v>
+        <v>525</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>514</v>
+        <v>526</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>515</v>
+        <v>527</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>516</v>
+        <v>528</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>517</v>
+        <v>529</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>518</v>
+        <v>530</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>519</v>
+        <v>531</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>520</v>
+        <v>532</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>521</v>
+        <v>533</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>522</v>
+        <v>534</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>523</v>
+        <v>535</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>524</v>
+        <v>536</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>525</v>
+        <v>537</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>526</v>
+        <v>538</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>527</v>
+        <v>539</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>528</v>
+        <v>540</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>529</v>
+        <v>541</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>530</v>
+        <v>542</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>531</v>
+        <v>543</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>532</v>
+        <v>544</v>
       </c>
     </row>
   </sheetData>
@@ -4004,34 +4061,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>442</v>
+        <v>454</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>443</v>
+        <v>455</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>183</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>430</v>
+        <v>442</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>431</v>
+        <v>443</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>434</v>
+        <v>446</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>435</v>
+        <v>447</v>
       </c>
     </row>
   </sheetData>
@@ -4049,34 +4106,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>536</v>
+        <v>548</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>537</v>
+        <v>549</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>538</v>
+        <v>550</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>539</v>
+        <v>551</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>540</v>
+        <v>552</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>541</v>
+        <v>553</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>434</v>
+        <v>446</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>435</v>
+        <v>447</v>
       </c>
     </row>
   </sheetData>
@@ -4094,74 +4151,74 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>150</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>168</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>183</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>545</v>
+        <v>557</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>546</v>
+        <v>558</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>547</v>
+        <v>559</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>548</v>
+        <v>560</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>170</v>
+        <v>176</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>172</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>549</v>
+        <v>561</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>550</v>
+        <v>562</v>
       </c>
     </row>
   </sheetData>
@@ -4179,146 +4236,146 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>250</v>
+        <v>258</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>251</v>
+        <v>259</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>183</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>552</v>
+        <v>564</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>553</v>
+        <v>565</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>187</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>554</v>
+        <v>566</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>555</v>
+        <v>567</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>233</v>
+        <v>241</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>299</v>
+        <v>307</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>556</v>
+        <v>568</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>557</v>
+        <v>569</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>558</v>
+        <v>570</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>559</v>
+        <v>571</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>560</v>
+        <v>572</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>561</v>
+        <v>573</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>562</v>
+        <v>574</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>563</v>
+        <v>575</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>564</v>
+        <v>576</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>565</v>
+        <v>577</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>566</v>
+        <v>578</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>567</v>
+        <v>579</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>568</v>
+        <v>580</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>569</v>
+        <v>581</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>570</v>
+        <v>582</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>571</v>
+        <v>583</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>572</v>
+        <v>584</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>573</v>
+        <v>585</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>574</v>
+        <v>586</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>575</v>
+        <v>587</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>576</v>
+        <v>588</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>577</v>
+        <v>589</v>
       </c>
     </row>
   </sheetData>
@@ -4336,90 +4393,90 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>579</v>
+        <v>591</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>580</v>
+        <v>592</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>581</v>
+        <v>593</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>582</v>
+        <v>594</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>442</v>
+        <v>454</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>443</v>
+        <v>455</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>430</v>
+        <v>442</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>431</v>
+        <v>443</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>583</v>
+        <v>595</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>584</v>
+        <v>596</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>585</v>
+        <v>597</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>586</v>
+        <v>598</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>587</v>
+        <v>599</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>588</v>
+        <v>600</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>589</v>
+        <v>601</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>590</v>
+        <v>602</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>434</v>
+        <v>446</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>435</v>
+        <v>447</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>591</v>
+        <v>603</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>592</v>
+        <v>604</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>593</v>
+        <v>605</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>594</v>
+        <v>606</v>
       </c>
     </row>
   </sheetData>
@@ -4443,30 +4500,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>597</v>
+        <v>609</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>599</v>
+        <v>610</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>601</v>
+        <v>612</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>603</v>
+        <v>614</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>598</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>600</v>
+        <v>611</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>602</v>
+        <v>613</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>604</v>
+        <v>615</v>
       </c>
     </row>
   </sheetData>
@@ -4484,130 +4541,130 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -4625,12 +4682,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -4640,7 +4697,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4648,210 +4705,226 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>174</v>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>177</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>179</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -4861,7 +4934,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B68"/>
+  <dimension ref="A1:B69"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4869,546 +4942,554 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>177</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>179</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>181</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>185</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>187</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>189</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>191</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>193</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>195</v>
+        <v>201</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>197</v>
+        <v>203</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>199</v>
+        <v>205</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>203</v>
+        <v>209</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>205</v>
+        <v>211</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>207</v>
+        <v>213</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>209</v>
+        <v>215</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>211</v>
+        <v>217</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>213</v>
+        <v>219</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>217</v>
+        <v>223</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>219</v>
+        <v>225</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>221</v>
+        <v>227</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>223</v>
+        <v>229</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>225</v>
+        <v>231</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>227</v>
+        <v>233</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>229</v>
+        <v>235</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>231</v>
+        <v>237</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>233</v>
+        <v>239</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>235</v>
+        <v>241</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>237</v>
+        <v>243</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>241</v>
+        <v>247</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>243</v>
+        <v>249</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>245</v>
+        <v>251</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>247</v>
+        <v>253</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>249</v>
+        <v>255</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>251</v>
+        <v>257</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>253</v>
+        <v>259</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>255</v>
+        <v>261</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>257</v>
+        <v>263</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>259</v>
+        <v>265</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>261</v>
+        <v>267</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>263</v>
+        <v>269</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>265</v>
+        <v>271</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>267</v>
+        <v>273</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>269</v>
+        <v>275</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>271</v>
+        <v>277</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>273</v>
+        <v>279</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>275</v>
+        <v>281</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>277</v>
+        <v>283</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>279</v>
+        <v>285</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="0">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>281</v>
+        <v>287</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="0">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="B54" t="s" s="0">
-        <v>283</v>
+        <v>289</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="0">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>285</v>
+        <v>291</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="0">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>287</v>
+        <v>293</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="0">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>289</v>
+        <v>295</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="0">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>291</v>
+        <v>297</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="0">
-        <v>149</v>
+        <v>298</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>150</v>
+        <v>299</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="0">
-        <v>292</v>
+        <v>155</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>293</v>
+        <v>156</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="0">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>295</v>
+        <v>301</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="0">
-        <v>296</v>
+        <v>302</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>297</v>
+        <v>303</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="0">
-        <v>298</v>
+        <v>304</v>
       </c>
       <c r="B63" t="s" s="0">
-        <v>299</v>
+        <v>305</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="0">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="B64" t="s" s="0">
-        <v>301</v>
+        <v>307</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="0">
-        <v>302</v>
+        <v>308</v>
       </c>
       <c r="B65" t="s" s="0">
-        <v>303</v>
+        <v>309</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s" s="0">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>305</v>
+        <v>311</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s" s="0">
-        <v>306</v>
+        <v>312</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>307</v>
+        <v>313</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s" s="0">
-        <v>308</v>
+        <v>314</v>
       </c>
       <c r="B68" t="s" s="0">
-        <v>309</v>
+        <v>315</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s" s="0">
+        <v>316</v>
+      </c>
+      <c r="B69" t="s" s="0">
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -5426,42 +5507,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>312</v>
+        <v>320</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>313</v>
+        <v>321</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>314</v>
+        <v>322</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>315</v>
+        <v>323</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>316</v>
+        <v>324</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>317</v>
+        <v>325</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>318</v>
+        <v>326</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>319</v>
+        <v>327</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>320</v>
+        <v>328</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>321</v>
+        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -5479,26 +5560,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>314</v>
+        <v>322</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>315</v>
+        <v>323</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>316</v>
+        <v>324</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>317</v>
+        <v>325</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>318</v>
+        <v>326</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>319</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -5516,37 +5597,37 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>327</v>
+        <v>335</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>328</v>
+        <v>336</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>329</v>
+        <v>337</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>330</v>
+        <v>338</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>331</v>
+        <v>339</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>332</v>
+        <v>340</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>182</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update sequence metadata templates to use updated field description
</commit_message>
<xml_diff>
--- a/atacseq/latest/atacseq.xlsx
+++ b/atacseq/latest/atacseq.xlsx
@@ -48,106 +48,112 @@
   <commentList>
     <comment ref="A1" authorId="1">
       <text>
-        <t>(Required) Unique HuBMAP or SenNet identifier of the sample (i.e., block,
-section or suspension) used to perform this assay. For example, for a RNAseq
-assay, the parent would be the suspension, whereas, for one of the imaging
-assays, the parent would be the tissue section. If an assay comes from multiple
-parent samples then this should be a comma separated list. Example:
-HBM386.ZGKG.235, HBM672.MKPK.442 or SNT232.UBHJ.322, SNT329.ALSK.102</t>
+        <t>(Required) The unique identifier from HuBMAP or SenNet for the sample (such as a
+block, section, or suspension) used to perform the assay. For instance, in an
+RNAseq assay, the parent sample would be the suspension, while in imaging
+assays, it would be the tissue section. If the assay is derived from multiple
+parent samples, this field should contain a comma-separated list of identifiers.
+Example: HBM386.ZGKG.235, HBM672.MKPK.442</t>
       </text>
     </comment>
     <comment ref="B1" authorId="1">
       <text>
-        <t>An internal field labs can use it to add whatever ID(s) they want or need for
-dataset validation and tracking. This could be a single ID (e.g.,
-"Visium_9OLC_A4_S1") or a delimited list of IDs (e.g., “9OL; 9OLC.A2;
-Visium_9OLC_A4_S1”). This field will not be accessible to anyone outside of the
-consortium and no effort will be made to check if IDs provided by one data
-provider are also used by another.</t>
+        <t>A locally assigned identifier provided by the data provider for the dataset. It
+is used to reference an external metadata record that may be maintained
+independently, enabling traceability and supporting provenance tracking.
+Example: Visium_9OLC_A4_S1</t>
       </text>
     </comment>
     <comment ref="C1" authorId="1">
       <text>
-        <t>(Required) DOI for the protocols.io page that describes the assay or sample
-procurement and preparation. For example for an imaging assay, the protocol
-might begin with staining of a section and finalize with the creation of an
-OME-TIFF file. In this case the protocol would include any image processing
-steps required to create the OME-TIFF file. Example:
-https://dx.doi.org/10.17504/protocols.io.eq2lyno9qvx9/v1.</t>
+        <t>(Required) The DOI for the protocols.io page that details the assay or the
+procedures used for sample procurement and preparation. For example, in the case
+of an imaging assay, the protocol may start with tissue section staining and end
+with the generation of an OME-TIFF file. The documented protocol should also
+include any image processing steps involved in producing the final OME-TIFF.
+Example: https://dx.doi.org/10.17504/protocols.io.eq2lyno9qvx9/v1</t>
       </text>
     </comment>
     <comment ref="D1" authorId="1">
       <text>
-        <t>(Required) The specific type of dataset being produced.</t>
+        <t>(Required) The specific type of dataset being produced. Example: RNAseq</t>
       </text>
     </comment>
     <comment ref="E1" authorId="1">
       <text>
-        <t>(Required) Analytes are the target molecules being measured with the assay.</t>
+        <t>(Required) The analyte class which is the target molecule that the assay is
+measuring. Example: DNA</t>
       </text>
     </comment>
     <comment ref="F1" authorId="1">
       <text>
-        <t>(Required) Specifies whether or not a specific molecule(s) is/are targeted for
-detection/measurement by the assay ("Yes" or "No"). The CODEX analyte is
-protein.</t>
+        <t>(Required) Indicates whether a specific molecule or set of molecules is targeted
+for detection or measurement by the assay. Example: Yes</t>
       </text>
     </comment>
     <comment ref="G1" authorId="1">
       <text>
-        <t>(Required) An acquisition instrument is the device that contains the signal
-detection hardware and signal processing software. Assays generate signals such
-as light of various intensities or color or signals representing the molecular
-mass.</t>
+        <t>(Required) The company that manufactures or supplies the acquisition instrument.
+An acquisition instrument is a device equipped with signal detection hardware
+and signal processing software. It captures signals produced by assays, such as
+variations in light intensity or color, or signals corresponding to molecular
+mass. If the instrument was custom-built or developed internally, enter
+"In-House". Example: Illumina</t>
       </text>
     </comment>
     <comment ref="H1" authorId="1">
       <text>
-        <t>(Required) Manufacturers of an acquisition instrument may offer various versions
-(models) of that instrument with different features or sensitivities.
-Differences in features or sensitivities may be relevant to processing or
-interpretation of the data.</t>
+        <t>(Required) The specific model of the acquisition instrument, as manufacturers
+often offer various versions with differing features or sensitivities. These
+differences may be relevant to the processing or interpretation of the data. If
+the instrument was custom-built or developed internally, enter "In-House". If
+the model is unknown, enter "Unknown". Example: HiSeq 4000</t>
       </text>
     </comment>
     <comment ref="I1" authorId="1">
       <text>
-        <t>(Required) How long was the source material (parent) stored, prior to this
-sample being processed.</t>
+        <t>(Required) The length of time the sample was stored prior to processing it. For
+assays performed on tissue sections, this refers to how long the tissue section
+(e.g., slide) was stored before the assay began (e.g., imaging). For assays
+performed on suspensions, such as sequencing, it refers to how long the
+suspension was stored before library construction started. Example: 12</t>
       </text>
     </comment>
     <comment ref="J1" authorId="1">
       <text>
-        <t>(Required) The time duration unit of measurement</t>
+        <t>(Required) The unit of measurement used to specify the source storage duration
+value. Example: hour</t>
       </text>
     </comment>
     <comment ref="K1" authorId="1">
       <text>
-        <t>The amount of time since the acquisition instrument was last serviced or
-calibrated. This provides a metric for assessing drift in data capture.</t>
+        <t>The length of time since the acquisition instrument was last serviced or
+calibrated. This provides a metric for assessing drift in data capture. Example:
+10</t>
       </text>
     </comment>
     <comment ref="L1" authorId="1">
       <text>
-        <t>The time unit of measurement</t>
+        <t>The unit of measurement used to specify the time since acquisition instrument
+calibration value. Example: month</t>
       </text>
     </comment>
     <comment ref="M1" authorId="1">
       <text>
-        <t>(Required) The path to the file with the ORCID IDs for all contributors of this
-dataset (e.g., "./extras/contributors.tsv" or "./contributors.tsv"). This is an
-internal metadata field that is just used for ingest.</t>
+        <t>(Required) The name of the file containing the ORCID IDs for all contributors to
+this dataset. Example: ./contributors.csv</t>
       </text>
     </comment>
     <comment ref="N1" authorId="1">
       <text>
-        <t>(Required) The top level directory containing the raw and/or processed data. For
-a single dataset upload this might be "." where as for a data upload containing
-multiple datasets, this would be the directory name for the respective dataset.
-For instance, if the data is within a directory called "TEST001-RK" use syntax
-"./TEST001-RK" for this field. If there are multiple directory levels, use the
-format "./TEST001-RK/Run1/Pass2" in which "Pass2" is the subdirectory where the
-single dataset's data is stored. This is an internal metadata field that is just
-used for ingest.</t>
+        <t>(Required) The top-level directory containing the raw and/or processed data. For
+a single dataset upload, this might be represented as ".", whereas for a data
+upload containing multiple datasets, this would be the directory name for the
+respective dataset. For example, if the data is within a directory named
+"TEST001-RK", use the syntax "./TEST001-RK" for this field. If there are
+multiple directory levels, use the format "./TEST001-RK/Run1/Pass2", where
+"Pass2" is the subdirectory where the single dataset's data is stored. This is
+an internal metadata field used solely for data ingestion. Example: ./TEST001-RK</t>
       </text>
     </comment>
     <comment ref="O1" authorId="1">
@@ -179,8 +185,10 @@
     </comment>
     <comment ref="R1" authorId="1">
       <text>
-        <t>(Required) Position in the read at which the UMI barcode starts. This should be
-included when constructing sequencing libraries with a non-commercial kit.</t>
+        <t>(Required) The position within a sequencing read where the Unique Molecular
+Identifier (UMI) sequence begins. UMIs are short, random nucleotide sequences
+added to DNA or RNA fragments during library preparation to uniquely tag each
+original molecule. If no UMI is used, enter "Not applicable". Example: 16</t>
       </text>
     </comment>
     <comment ref="S1" authorId="1">
@@ -371,8 +379,8 @@
     </comment>
     <comment ref="AU1" authorId="1">
       <text>
-        <t>(Required) The string that serves as the definitive identifier for the metadata
-schema version and is readily interpretable by computers for data validation and
+        <t>(Required) The unique string identifier for the metadata specification version,
+which is easily interpretable by computers for purposes of data validation and
 processing. Example: 22bc762a-5020-419d-b170-24253ed9e8d9</t>
       </text>
     </comment>
@@ -381,7 +389,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="616">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="659">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -407,34 +415,172 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000264</t>
   </si>
   <si>
+    <t>COMET</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000458</t>
+  </si>
+  <si>
+    <t>Visium (no probes)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000302</t>
+  </si>
+  <si>
+    <t>DESI</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000204</t>
+  </si>
+  <si>
+    <t>Confocal</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000206</t>
+  </si>
+  <si>
+    <t>Stereo-seq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000385</t>
+  </si>
+  <si>
+    <t>Visium (with probes)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000303</t>
+  </si>
+  <si>
+    <t>Molecular Cartography</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000217</t>
+  </si>
+  <si>
+    <t>DBiT-seq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000428</t>
+  </si>
+  <si>
+    <t>Seq-Scope</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000390</t>
+  </si>
+  <si>
+    <t>CosMx Transcriptomics</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000218</t>
+  </si>
+  <si>
+    <t>CyCIF</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000200</t>
+  </si>
+  <si>
+    <t>Light Sheet</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000168</t>
+  </si>
+  <si>
+    <t>seqFISH</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000397</t>
+  </si>
+  <si>
+    <t>ATACseq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000309</t>
+  </si>
+  <si>
+    <t>CosMx Proteomics</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000435</t>
+  </si>
+  <si>
+    <t>Singular Genomics G4X</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000429</t>
+  </si>
+  <si>
+    <t>Visium HD</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000451</t>
+  </si>
+  <si>
+    <t>MERFISH</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000221</t>
+  </si>
+  <si>
+    <t>10X Multiome</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000215</t>
+  </si>
+  <si>
+    <t>4i</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000447</t>
+  </si>
+  <si>
+    <t>PhenoCycler</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000199</t>
+  </si>
+  <si>
+    <t>Second Harmonic Generation (SHG)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000208</t>
+  </si>
+  <si>
+    <t>Thick section Multiphoton MxIF</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000207</t>
+  </si>
+  <si>
+    <t>CyTOF</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000407</t>
+  </si>
+  <si>
+    <t>Olink</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000441</t>
+  </si>
+  <si>
     <t>MIBI</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000172</t>
   </si>
   <si>
-    <t>Visium (no probes)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000302</t>
-  </si>
-  <si>
-    <t>DESI</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000204</t>
-  </si>
-  <si>
     <t>Auto-fluorescence</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000205</t>
   </si>
   <si>
-    <t>Confocal</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000206</t>
+    <t>FACS</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000440</t>
   </si>
   <si>
     <t>Xenium</t>
@@ -443,36 +589,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000219</t>
   </si>
   <si>
-    <t>Stereo-seq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000385</t>
-  </si>
-  <si>
-    <t>Visium (with probes)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000303</t>
-  </si>
-  <si>
-    <t>Molecular Cartography</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000217</t>
-  </si>
-  <si>
-    <t>CosMx</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000218</t>
-  </si>
-  <si>
-    <t>DBiT-seq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000428</t>
-  </si>
-  <si>
     <t>SIMS</t>
   </si>
   <si>
@@ -503,16 +619,10 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000328</t>
   </si>
   <si>
-    <t>CyCIF</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000200</t>
-  </si>
-  <si>
-    <t>Light Sheet</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000168</t>
+    <t>Pixel-seqV2</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000450</t>
   </si>
   <si>
     <t>MALDI</t>
@@ -521,30 +631,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000201</t>
   </si>
   <si>
-    <t>seqFISH</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000397</t>
-  </si>
-  <si>
     <t>2D Imaging Mass Cytometry</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000296</t>
   </si>
   <si>
-    <t>ATACseq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000309</t>
-  </si>
-  <si>
-    <t>CosMx Proteomics</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000435</t>
-  </si>
-  <si>
     <t>Histology</t>
   </si>
   <si>
@@ -575,18 +667,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000310</t>
   </si>
   <si>
-    <t>Singular Genomics G4X</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000429</t>
-  </si>
-  <si>
-    <t>MERFISH</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000221</t>
-  </si>
-  <si>
     <t>LC-MS</t>
   </si>
   <si>
@@ -599,12 +679,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000312</t>
   </si>
   <si>
-    <t>10X Multiome</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000215</t>
-  </si>
-  <si>
     <t>GeoMx (nCounter)</t>
   </si>
   <si>
@@ -617,34 +691,16 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000311</t>
   </si>
   <si>
-    <t>PhenoCycler</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000199</t>
-  </si>
-  <si>
-    <t>Second Harmonic Generation (SHG)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000208</t>
-  </si>
-  <si>
-    <t>Thick section Multiphoton MxIF</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000207</t>
-  </si>
-  <si>
     <t>MS Lipidomics</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000405</t>
   </si>
   <si>
-    <t>CyTOF</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000407</t>
+    <t>MPLEx</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000448</t>
   </si>
   <si>
     <t>analyte_class</t>
@@ -908,12 +964,24 @@
     <t>https://identifiers.org/RRID:SCR_023603</t>
   </si>
   <si>
+    <t>Cytek Biosciences</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027071</t>
+  </si>
+  <si>
     <t>10x Genomics</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_023672</t>
   </si>
   <si>
+    <t>Microscopes International</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027094</t>
+  </si>
+  <si>
     <t>Hamamatsu</t>
   </si>
   <si>
@@ -1061,6 +1129,12 @@
     <t>https://identifiers.org/RRID:SCR_019916</t>
   </si>
   <si>
+    <t>uScopeHXII-20</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027101</t>
+  </si>
+  <si>
     <t>Custom: Multiphoton</t>
   </si>
   <si>
@@ -1139,6 +1213,12 @@
     <t>https://identifiers.org/RRID:SCR_016381</t>
   </si>
   <si>
+    <t>Axio Zoom.V16</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027090</t>
+  </si>
+  <si>
     <t>Digital Spatial Profiler</t>
   </si>
   <si>
@@ -1175,6 +1255,12 @@
     <t>https://identifiers.org/RRID:SCR_023694</t>
   </si>
   <si>
+    <t>Cytek Northern Lights</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027072</t>
+  </si>
+  <si>
     <t>IN Cell Analyzer 2200</t>
   </si>
   <si>
@@ -1265,6 +1351,9 @@
     <t>https://identifiers.org/RRID:SCR_023618</t>
   </si>
   <si>
+    <t>https://identifiers.org/RRID:SCR_027323</t>
+  </si>
+  <si>
     <t>MERSCOPE</t>
   </si>
   <si>
@@ -1289,6 +1378,18 @@
     <t>https://identifiers.org/RRID:SCR_016386</t>
   </si>
   <si>
+    <t>solariX</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027095</t>
+  </si>
+  <si>
+    <t>Panoramic 150 Digital Scanner</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027467</t>
+  </si>
+  <si>
     <t>Aperio AT2</t>
   </si>
   <si>
@@ -1301,6 +1402,12 @@
     <t>https://identifiers.org/RRID:SCR_023613</t>
   </si>
   <si>
+    <t>Biomark HD</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_022658</t>
+  </si>
+  <si>
     <t>NanoZoomer S60</t>
   </si>
   <si>
@@ -1325,6 +1432,12 @@
     <t>https://identifiers.org/RRID:SCR_020927</t>
   </si>
   <si>
+    <t>Juno System</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027198</t>
+  </si>
+  <si>
     <t>Q Exactive HF</t>
   </si>
   <si>
@@ -1733,6 +1846,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000260</t>
   </si>
   <si>
+    <t>10x Genomics; Chromium Single Cell 3ʹ GEM, Library &amp; Gel Bead Kit v3, 16 rxns; PN 1000075</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000460</t>
+  </si>
+  <si>
     <t>10X Genomics; Chromium Single Cell 3' Library &amp; Gel Bead Kit, 4 rxns; PN 120267</t>
   </si>
   <si>
@@ -1766,6 +1885,12 @@
     <t>sample_indexing_kit</t>
   </si>
   <si>
+    <t>10x Genomics; Chromium i7 Multiplex Kit, 96 rxns; PN 120262</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000461</t>
+  </si>
+  <si>
     <t>Illumina; TruSeq RNA CD Index Plate (96 Indexes, 96 Samples); PN 20019792</t>
   </si>
   <si>
@@ -1988,6 +2113,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000313</t>
   </si>
   <si>
+    <t>Illumina; NovaSeq 6000 SP Reagent v1.5 Kit (300 Cycles); PN 20028400</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000459</t>
+  </si>
+  <si>
     <t>Illumina; NovaSeq 6000 S4 Reagent v1.5 Kit (200 Cycles); PN 20028313</t>
   </si>
   <si>
@@ -2168,6 +2299,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000373</t>
   </si>
   <si>
+    <t>10x Genomics; Chromium Single Cell B Chip Kit, 16 rxns; PN 1000074</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000462</t>
+  </si>
+  <si>
     <t>10x Genomics; Chromium GEM-X Single Cell 3' Kit v4, 16 rxns; PN 1000691</t>
   </si>
   <si>
@@ -2222,7 +2359,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-06-10T14:22:23-07:00</t>
+    <t>2025-10-17T11:50:25-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -2412,147 +2549,147 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>124</v>
+        <v>140</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>181</v>
+        <v>201</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>318</v>
+        <v>353</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>319</v>
+        <v>354</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>330</v>
+        <v>365</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>331</v>
+        <v>366</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>332</v>
+        <v>367</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>333</v>
+        <v>368</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>334</v>
+        <v>369</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>341</v>
+        <v>376</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>346</v>
+        <v>381</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>352</v>
+        <v>387</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>354</v>
+        <v>389</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>355</v>
+        <v>390</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>359</v>
+        <v>394</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>370</v>
+        <v>405</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>371</v>
+        <v>406</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>372</v>
+        <v>407</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>373</v>
+        <v>408</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>374</v>
+        <v>409</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>379</v>
+        <v>414</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>380</v>
+        <v>415</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>381</v>
+        <v>416</v>
       </c>
       <c r="AD1" t="s" s="1">
-        <v>382</v>
+        <v>417</v>
       </c>
       <c r="AE1" t="s" s="1">
-        <v>389</v>
+        <v>424</v>
       </c>
       <c r="AF1" t="s" s="1">
-        <v>394</v>
+        <v>429</v>
       </c>
       <c r="AG1" t="s" s="1">
-        <v>395</v>
+        <v>430</v>
       </c>
       <c r="AH1" t="s" s="1">
-        <v>460</v>
+        <v>497</v>
       </c>
       <c r="AI1" t="s" s="1">
-        <v>491</v>
+        <v>530</v>
       </c>
       <c r="AJ1" t="s" s="1">
-        <v>492</v>
+        <v>531</v>
       </c>
       <c r="AK1" t="s" s="1">
-        <v>493</v>
+        <v>532</v>
       </c>
       <c r="AL1" t="s" s="1">
-        <v>494</v>
+        <v>533</v>
       </c>
       <c r="AM1" t="s" s="1">
-        <v>545</v>
+        <v>586</v>
       </c>
       <c r="AN1" t="s" s="1">
-        <v>546</v>
+        <v>587</v>
       </c>
       <c r="AO1" t="s" s="1">
-        <v>547</v>
+        <v>588</v>
       </c>
       <c r="AP1" t="s" s="1">
-        <v>554</v>
+        <v>595</v>
       </c>
       <c r="AQ1" t="s" s="1">
-        <v>555</v>
+        <v>596</v>
       </c>
       <c r="AR1" t="s" s="1">
-        <v>556</v>
+        <v>597</v>
       </c>
       <c r="AS1" t="s" s="1">
-        <v>563</v>
+        <v>604</v>
       </c>
       <c r="AT1" t="s" s="1">
-        <v>590</v>
+        <v>631</v>
       </c>
       <c r="AU1" t="s" s="1">
-        <v>607</v>
+        <v>650</v>
       </c>
     </row>
     <row r="2">
       <c r="D2" t="s" s="5">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="AU2" t="s" s="48">
-        <v>608</v>
+        <v>651</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="36">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$42</formula1>
+      <formula1>'dataset_type'!$A$1:$A$50</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'analyte_class'!$A$1:$A$16</formula1>
@@ -2561,10 +2698,10 @@
       <formula1>'is_targeted'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_vendor'!$A$1:$A$28</formula1>
+      <formula1>'acquisition_instrument_vendor'!$A$1:$A$30</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$69</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$77</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -2638,10 +2775,10 @@
       <formula2>2147483647</formula2>
     </dataValidation>
     <dataValidation type="list" sqref="AG2:AG1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'library_preparation_kit'!$A$1:$A$32</formula1>
+      <formula1>'library_preparation_kit'!$A$1:$A$33</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AH2:AH1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'sample_indexing_kit'!$A$1:$A$17</formula1>
+      <formula1>'sample_indexing_kit'!$A$1:$A$18</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AJ2:AJ1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'is_technical_replicate'!$A$1:$A$2</formula1>
@@ -2651,7 +2788,7 @@
       <formula2>2147483647</formula2>
     </dataValidation>
     <dataValidation type="list" sqref="AL2:AL1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'sequencing_reagent_kit'!$A$1:$A$26</formula1>
+      <formula1>'sequencing_reagent_kit'!$A$1:$A$27</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AN2:AN1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'transposition_reagent_kit'!$A$1:$A$4</formula1>
@@ -2666,7 +2803,7 @@
       <formula1>'preparation_instrument_model'!$A$1:$A$18</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AT2:AT1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'preparation_instrument_kit'!$A$1:$A$11</formula1>
+      <formula1>'preparation_instrument_kit'!$A$1:$A$12</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -2685,26 +2822,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>342</v>
+        <v>377</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>343</v>
+        <v>378</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>191</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>344</v>
+        <v>379</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>345</v>
+        <v>380</v>
       </c>
     </row>
   </sheetData>
@@ -2722,32 +2859,32 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>347</v>
+        <v>382</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>348</v>
+        <v>383</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>349</v>
+        <v>384</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>350</v>
+        <v>385</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>351</v>
+        <v>386</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>190</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -2765,22 +2902,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>335</v>
+        <v>370</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>348</v>
+        <v>383</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>353</v>
+        <v>388</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>190</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -2798,26 +2935,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>342</v>
+        <v>377</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>343</v>
+        <v>378</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>191</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>344</v>
+        <v>379</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>345</v>
+        <v>380</v>
       </c>
     </row>
   </sheetData>
@@ -2835,27 +2972,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>336</v>
+        <v>371</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>356</v>
+        <v>391</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>357</v>
+        <v>392</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>358</v>
+        <v>393</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>190</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -2873,42 +3010,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>360</v>
+        <v>395</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>361</v>
+        <v>396</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>362</v>
+        <v>397</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>363</v>
+        <v>398</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>364</v>
+        <v>399</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>365</v>
+        <v>400</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>366</v>
+        <v>401</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>367</v>
+        <v>402</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>368</v>
+        <v>403</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>369</v>
+        <v>404</v>
       </c>
     </row>
   </sheetData>
@@ -2926,18 +3063,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>375</v>
+        <v>410</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>376</v>
+        <v>411</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>377</v>
+        <v>412</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>378</v>
+        <v>413</v>
       </c>
     </row>
   </sheetData>
@@ -2955,18 +3092,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>375</v>
+        <v>410</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>376</v>
+        <v>411</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>377</v>
+        <v>412</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>378</v>
+        <v>413</v>
       </c>
     </row>
   </sheetData>
@@ -2984,26 +3121,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>383</v>
+        <v>418</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>384</v>
+        <v>419</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>385</v>
+        <v>420</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>386</v>
+        <v>421</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>387</v>
+        <v>422</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>388</v>
+        <v>423</v>
       </c>
     </row>
   </sheetData>
@@ -3021,18 +3158,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>390</v>
+        <v>425</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>391</v>
+        <v>426</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>392</v>
+        <v>427</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>393</v>
+        <v>428</v>
       </c>
     </row>
   </sheetData>
@@ -3042,7 +3179,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3384,6 +3521,70 @@
         <v>87</v>
       </c>
     </row>
+    <row r="43">
+      <c r="A43" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="B43" t="s" s="0">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="B44" t="s" s="0">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="0">
+        <v>92</v>
+      </c>
+      <c r="B45" t="s" s="0">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>94</v>
+      </c>
+      <c r="B46" t="s" s="0">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
+        <v>96</v>
+      </c>
+      <c r="B47" t="s" s="0">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="0">
+        <v>98</v>
+      </c>
+      <c r="B48" t="s" s="0">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="0">
+        <v>100</v>
+      </c>
+      <c r="B49" t="s" s="0">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="0">
+        <v>102</v>
+      </c>
+      <c r="B50" t="s" s="0">
+        <v>103</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -3391,7 +3592,7 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3399,258 +3600,266 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>396</v>
+        <v>431</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>397</v>
+        <v>432</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>398</v>
+        <v>433</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>399</v>
+        <v>434</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>400</v>
+        <v>435</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>401</v>
+        <v>436</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>402</v>
+        <v>437</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>403</v>
+        <v>438</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>404</v>
+        <v>439</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>405</v>
+        <v>440</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>406</v>
+        <v>441</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>407</v>
+        <v>442</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>408</v>
+        <v>443</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>409</v>
+        <v>444</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>410</v>
+        <v>445</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>411</v>
+        <v>446</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>412</v>
+        <v>447</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>413</v>
+        <v>448</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>414</v>
+        <v>449</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>415</v>
+        <v>450</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>416</v>
+        <v>451</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>417</v>
+        <v>452</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>418</v>
+        <v>453</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>419</v>
+        <v>454</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>420</v>
+        <v>455</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>421</v>
+        <v>456</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>422</v>
+        <v>457</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>423</v>
+        <v>458</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>424</v>
+        <v>459</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>425</v>
+        <v>460</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>426</v>
+        <v>461</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>427</v>
+        <v>462</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>428</v>
+        <v>463</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>429</v>
+        <v>464</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>430</v>
+        <v>465</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>431</v>
+        <v>466</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>432</v>
+        <v>467</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>433</v>
+        <v>468</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>434</v>
+        <v>469</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>435</v>
+        <v>470</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>436</v>
+        <v>471</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>437</v>
+        <v>472</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>438</v>
+        <v>473</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>439</v>
+        <v>474</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>440</v>
+        <v>475</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>441</v>
+        <v>476</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>442</v>
+        <v>477</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>443</v>
+        <v>478</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>444</v>
+        <v>479</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>445</v>
+        <v>480</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>446</v>
+        <v>481</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>447</v>
+        <v>482</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>448</v>
+        <v>483</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>449</v>
+        <v>484</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>450</v>
+        <v>485</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>451</v>
+        <v>486</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>452</v>
+        <v>487</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>453</v>
+        <v>488</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>454</v>
+        <v>489</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>455</v>
+        <v>490</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>456</v>
+        <v>491</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>457</v>
+        <v>492</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>458</v>
+        <v>493</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>459</v>
+        <v>494</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s" s="0">
+        <v>495</v>
+      </c>
+      <c r="B33" t="s" s="0">
+        <v>496</v>
       </c>
     </row>
   </sheetData>
@@ -3660,7 +3869,7 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3668,138 +3877,146 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>461</v>
+        <v>498</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>462</v>
+        <v>499</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>190</v>
+        <v>500</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>191</v>
+        <v>501</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>463</v>
+        <v>210</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>464</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>465</v>
+        <v>502</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>466</v>
+        <v>503</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>467</v>
+        <v>504</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>468</v>
+        <v>505</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>469</v>
+        <v>506</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>470</v>
+        <v>507</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>471</v>
+        <v>508</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>472</v>
+        <v>509</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>473</v>
+        <v>510</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>474</v>
+        <v>511</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>475</v>
+        <v>512</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>476</v>
+        <v>513</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>446</v>
+        <v>514</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>447</v>
+        <v>515</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>477</v>
+        <v>481</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>478</v>
+        <v>482</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>479</v>
+        <v>516</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>480</v>
+        <v>517</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>481</v>
+        <v>518</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>482</v>
+        <v>519</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>483</v>
+        <v>520</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>484</v>
+        <v>521</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>485</v>
+        <v>522</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>486</v>
+        <v>523</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>487</v>
+        <v>524</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>488</v>
+        <v>525</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>489</v>
+        <v>526</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>490</v>
+        <v>527</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="0">
+        <v>528</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>529</v>
       </c>
     </row>
   </sheetData>
@@ -3817,12 +4034,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>122</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>123</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -3832,7 +4049,7 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3840,210 +4057,218 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>495</v>
+        <v>534</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>496</v>
+        <v>535</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>497</v>
+        <v>536</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>498</v>
+        <v>537</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>499</v>
+        <v>538</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>500</v>
+        <v>539</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>501</v>
+        <v>540</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>502</v>
+        <v>541</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>503</v>
+        <v>542</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>504</v>
+        <v>543</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>505</v>
+        <v>544</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>506</v>
+        <v>545</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>507</v>
+        <v>546</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>508</v>
+        <v>547</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>509</v>
+        <v>548</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>510</v>
+        <v>549</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>511</v>
+        <v>550</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>512</v>
+        <v>551</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>513</v>
+        <v>552</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>514</v>
+        <v>553</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>515</v>
+        <v>554</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>516</v>
+        <v>555</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>517</v>
+        <v>556</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>518</v>
+        <v>557</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>519</v>
+        <v>558</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>520</v>
+        <v>559</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>521</v>
+        <v>560</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>522</v>
+        <v>561</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>523</v>
+        <v>562</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>524</v>
+        <v>563</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>446</v>
+        <v>481</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>447</v>
+        <v>482</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>525</v>
+        <v>564</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>526</v>
+        <v>565</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>527</v>
+        <v>566</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>528</v>
+        <v>567</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>529</v>
+        <v>568</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>530</v>
+        <v>569</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>531</v>
+        <v>570</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>532</v>
+        <v>571</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>533</v>
+        <v>572</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>534</v>
+        <v>573</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>535</v>
+        <v>574</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>536</v>
+        <v>575</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>537</v>
+        <v>576</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>538</v>
+        <v>577</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>539</v>
+        <v>578</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>540</v>
+        <v>579</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>541</v>
+        <v>580</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>542</v>
+        <v>581</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>543</v>
+        <v>582</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>544</v>
+        <v>583</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>584</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>585</v>
       </c>
     </row>
   </sheetData>
@@ -4061,34 +4286,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>454</v>
+        <v>491</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>455</v>
+        <v>492</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>191</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>442</v>
+        <v>477</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>443</v>
+        <v>478</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>446</v>
+        <v>481</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>447</v>
+        <v>482</v>
       </c>
     </row>
   </sheetData>
@@ -4106,34 +4331,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>548</v>
+        <v>589</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>549</v>
+        <v>590</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>550</v>
+        <v>591</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>551</v>
+        <v>592</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>552</v>
+        <v>593</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>553</v>
+        <v>594</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>446</v>
+        <v>481</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>447</v>
+        <v>482</v>
       </c>
     </row>
   </sheetData>
@@ -4151,74 +4376,74 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>156</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>173</v>
+        <v>189</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>174</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>191</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>129</v>
+        <v>145</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>130</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>557</v>
+        <v>598</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>558</v>
+        <v>599</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>559</v>
+        <v>600</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>560</v>
+        <v>601</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>175</v>
+        <v>193</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>176</v>
+        <v>194</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>177</v>
+        <v>197</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>178</v>
+        <v>198</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>561</v>
+        <v>602</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>562</v>
+        <v>603</v>
       </c>
     </row>
   </sheetData>
@@ -4236,146 +4461,146 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>258</v>
+        <v>282</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>259</v>
+        <v>283</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>191</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>564</v>
+        <v>605</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>565</v>
+        <v>606</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>194</v>
+        <v>214</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>195</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>566</v>
+        <v>607</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>567</v>
+        <v>608</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>240</v>
+        <v>262</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>241</v>
+        <v>263</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>306</v>
+        <v>339</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>307</v>
+        <v>340</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>568</v>
+        <v>609</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>569</v>
+        <v>610</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>570</v>
+        <v>611</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>571</v>
+        <v>612</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>572</v>
+        <v>613</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>573</v>
+        <v>614</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>574</v>
+        <v>615</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>575</v>
+        <v>616</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>576</v>
+        <v>617</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>577</v>
+        <v>618</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>578</v>
+        <v>619</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>579</v>
+        <v>620</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>580</v>
+        <v>621</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>581</v>
+        <v>622</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>582</v>
+        <v>623</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>583</v>
+        <v>624</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>584</v>
+        <v>625</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>585</v>
+        <v>626</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>586</v>
+        <v>627</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>587</v>
+        <v>628</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>588</v>
+        <v>629</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>589</v>
+        <v>630</v>
       </c>
     </row>
   </sheetData>
@@ -4385,7 +4610,7 @@
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4393,90 +4618,98 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>591</v>
+        <v>632</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>592</v>
+        <v>633</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>593</v>
+        <v>634</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>594</v>
+        <v>635</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>454</v>
+        <v>491</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>455</v>
+        <v>492</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>442</v>
+        <v>636</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>443</v>
+        <v>637</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>595</v>
+        <v>477</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>596</v>
+        <v>478</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>597</v>
+        <v>638</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>598</v>
+        <v>639</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>599</v>
+        <v>640</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>600</v>
+        <v>641</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>601</v>
+        <v>642</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>602</v>
+        <v>643</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>446</v>
+        <v>644</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>447</v>
+        <v>645</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>603</v>
+        <v>481</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>604</v>
+        <v>482</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>605</v>
+        <v>646</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>606</v>
+        <v>647</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>648</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>649</v>
       </c>
     </row>
   </sheetData>
@@ -4500,30 +4733,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>609</v>
+        <v>652</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>610</v>
+        <v>653</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>612</v>
+        <v>655</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>614</v>
+        <v>657</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>611</v>
+        <v>654</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>613</v>
+        <v>656</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>615</v>
+        <v>658</v>
       </c>
     </row>
   </sheetData>
@@ -4541,130 +4774,130 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>90</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>92</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>94</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>96</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>98</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>100</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>102</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>104</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>106</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>108</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>110</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>112</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>114</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>115</v>
+        <v>131</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>116</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>118</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>120</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -4682,12 +4915,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>122</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>123</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -4697,7 +4930,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4705,226 +4938,242 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>125</v>
+        <v>141</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>126</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>127</v>
+        <v>143</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>128</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>129</v>
+        <v>145</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>130</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>131</v>
+        <v>147</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>132</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>133</v>
+        <v>149</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>134</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>135</v>
+        <v>151</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>136</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>137</v>
+        <v>153</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>138</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>139</v>
+        <v>155</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>140</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>141</v>
+        <v>157</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>142</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>143</v>
+        <v>159</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>144</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>145</v>
+        <v>161</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>146</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>147</v>
+        <v>163</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>148</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>150</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>151</v>
+        <v>167</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>152</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>153</v>
+        <v>169</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>154</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>156</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>157</v>
+        <v>173</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>158</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>159</v>
+        <v>175</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>160</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>161</v>
+        <v>177</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>162</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>163</v>
+        <v>179</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>164</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>165</v>
+        <v>181</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>166</v>
+        <v>182</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>167</v>
+        <v>183</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>168</v>
+        <v>184</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>170</v>
+        <v>186</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>171</v>
+        <v>187</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>172</v>
+        <v>188</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>173</v>
+        <v>189</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>174</v>
+        <v>190</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>175</v>
+        <v>191</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>176</v>
+        <v>192</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>177</v>
+        <v>193</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>178</v>
+        <v>194</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>180</v>
+        <v>196</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>197</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>199</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -4934,7 +5183,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B69"/>
+  <dimension ref="A1:B77"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4942,554 +5191,618 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>182</v>
+        <v>202</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>183</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>184</v>
+        <v>204</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>185</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>186</v>
+        <v>206</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>187</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>188</v>
+        <v>208</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>189</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>191</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>192</v>
+        <v>212</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>193</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>194</v>
+        <v>214</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>195</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>196</v>
+        <v>216</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>197</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>198</v>
+        <v>218</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>199</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>201</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>202</v>
+        <v>222</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>203</v>
+        <v>223</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>204</v>
+        <v>224</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>205</v>
+        <v>225</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>206</v>
+        <v>226</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>207</v>
+        <v>227</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>208</v>
+        <v>228</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>209</v>
+        <v>229</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>210</v>
+        <v>230</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>211</v>
+        <v>231</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>212</v>
+        <v>232</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>213</v>
+        <v>233</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>214</v>
+        <v>234</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>215</v>
+        <v>235</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>216</v>
+        <v>236</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>217</v>
+        <v>237</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>218</v>
+        <v>238</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>219</v>
+        <v>239</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>220</v>
+        <v>240</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>221</v>
+        <v>241</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>222</v>
+        <v>242</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>223</v>
+        <v>243</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>224</v>
+        <v>244</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>225</v>
+        <v>245</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>226</v>
+        <v>246</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>227</v>
+        <v>247</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>228</v>
+        <v>248</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>229</v>
+        <v>249</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>230</v>
+        <v>250</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>231</v>
+        <v>251</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>232</v>
+        <v>252</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>233</v>
+        <v>253</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>234</v>
+        <v>254</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>235</v>
+        <v>255</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>236</v>
+        <v>256</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>237</v>
+        <v>257</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>238</v>
+        <v>258</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>239</v>
+        <v>259</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>240</v>
+        <v>260</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>241</v>
+        <v>261</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>242</v>
+        <v>262</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>243</v>
+        <v>263</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>244</v>
+        <v>264</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>245</v>
+        <v>265</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>246</v>
+        <v>266</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>247</v>
+        <v>267</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>248</v>
+        <v>268</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>249</v>
+        <v>269</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>251</v>
+        <v>271</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>252</v>
+        <v>272</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>253</v>
+        <v>273</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>254</v>
+        <v>274</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>255</v>
+        <v>275</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>256</v>
+        <v>276</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>257</v>
+        <v>277</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>258</v>
+        <v>278</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>259</v>
+        <v>279</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>261</v>
+        <v>281</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>262</v>
+        <v>282</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>263</v>
+        <v>283</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>264</v>
+        <v>284</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>265</v>
+        <v>285</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>266</v>
+        <v>286</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>267</v>
+        <v>287</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>268</v>
+        <v>288</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>269</v>
+        <v>289</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>270</v>
+        <v>290</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>271</v>
+        <v>291</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>272</v>
+        <v>292</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>273</v>
+        <v>293</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>274</v>
+        <v>294</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>275</v>
+        <v>295</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>277</v>
+        <v>297</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>279</v>
+        <v>299</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>280</v>
+        <v>300</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>281</v>
+        <v>301</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>282</v>
+        <v>302</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>283</v>
+        <v>303</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>284</v>
+        <v>304</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>285</v>
+        <v>305</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="0">
-        <v>286</v>
+        <v>306</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>287</v>
+        <v>307</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="0">
-        <v>288</v>
+        <v>308</v>
       </c>
       <c r="B54" t="s" s="0">
-        <v>289</v>
+        <v>309</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="0">
-        <v>290</v>
+        <v>310</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>291</v>
+        <v>311</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="0">
-        <v>292</v>
+        <v>312</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>293</v>
+        <v>313</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="0">
-        <v>294</v>
+        <v>314</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>295</v>
+        <v>315</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="0">
-        <v>296</v>
+        <v>316</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>297</v>
+        <v>317</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="0">
-        <v>298</v>
+        <v>318</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>299</v>
+        <v>319</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="0">
-        <v>155</v>
+        <v>68</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>156</v>
+        <v>320</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="0">
-        <v>300</v>
+        <v>321</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>301</v>
+        <v>322</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="0">
-        <v>302</v>
+        <v>323</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>303</v>
+        <v>324</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="0">
-        <v>304</v>
+        <v>325</v>
       </c>
       <c r="B63" t="s" s="0">
-        <v>305</v>
+        <v>326</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="0">
-        <v>306</v>
+        <v>171</v>
       </c>
       <c r="B64" t="s" s="0">
-        <v>307</v>
+        <v>172</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="0">
-        <v>308</v>
+        <v>327</v>
       </c>
       <c r="B65" t="s" s="0">
-        <v>309</v>
+        <v>328</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s" s="0">
-        <v>310</v>
+        <v>329</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>311</v>
+        <v>330</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s" s="0">
-        <v>312</v>
+        <v>331</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>313</v>
+        <v>332</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s" s="0">
-        <v>314</v>
+        <v>333</v>
       </c>
       <c r="B68" t="s" s="0">
-        <v>315</v>
+        <v>334</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s" s="0">
-        <v>316</v>
+        <v>335</v>
       </c>
       <c r="B69" t="s" s="0">
-        <v>317</v>
+        <v>336</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s" s="0">
+        <v>337</v>
+      </c>
+      <c r="B70" t="s" s="0">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s" s="0">
+        <v>339</v>
+      </c>
+      <c r="B71" t="s" s="0">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s" s="0">
+        <v>341</v>
+      </c>
+      <c r="B72" t="s" s="0">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s" s="0">
+        <v>343</v>
+      </c>
+      <c r="B73" t="s" s="0">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s" s="0">
+        <v>345</v>
+      </c>
+      <c r="B74" t="s" s="0">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s" s="0">
+        <v>347</v>
+      </c>
+      <c r="B75" t="s" s="0">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s" s="0">
+        <v>349</v>
+      </c>
+      <c r="B76" t="s" s="0">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s" s="0">
+        <v>351</v>
+      </c>
+      <c r="B77" t="s" s="0">
+        <v>352</v>
       </c>
     </row>
   </sheetData>
@@ -5507,42 +5820,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>320</v>
+        <v>355</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>321</v>
+        <v>356</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>322</v>
+        <v>357</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>323</v>
+        <v>358</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>324</v>
+        <v>359</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>325</v>
+        <v>360</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>326</v>
+        <v>361</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>327</v>
+        <v>362</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>328</v>
+        <v>363</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>329</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>
@@ -5560,26 +5873,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>322</v>
+        <v>357</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>323</v>
+        <v>358</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>324</v>
+        <v>359</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>325</v>
+        <v>360</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>326</v>
+        <v>361</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>327</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -5597,37 +5910,37 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>335</v>
+        <v>370</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>336</v>
+        <v>371</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>337</v>
+        <v>372</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>338</v>
+        <v>373</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>339</v>
+        <v>374</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>340</v>
+        <v>375</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>190</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Re-update Sequencing metadata templates to use updated field description
Closes #110
</commit_message>
<xml_diff>
--- a/atacseq/latest/atacseq.xlsx
+++ b/atacseq/latest/atacseq.xlsx
@@ -158,29 +158,30 @@
     </comment>
     <comment ref="O1" authorId="1">
       <text>
-        <t>(Required) Positions in the read at which the cell or capture spot barcodes
-start. Cell and capture spot barcodes are, for example, 3 x 8 bp sequences that
-are spaced by constant sequences (the offsets). First barcode at position 0,
-then 38, then 76. This should be included when constructing sequencing libraries
-with a non-commercial kit.</t>
+        <t>(Required) The position within a sequencing read where a barcode sequence
+begins. In sequencing libraries, barcodes—short DNA sequences used to tag
+individual cells or molecules—are often arranged in a pattern where each barcode
+is separated by a constant sequence of known length. These constant sequences
+create predictable spacing between barcodes, known as offsets. For example, if
+barcodes are 8 base pairs (bp) long and separated by 30 bp constant regions, the
+barcodes might start at positions 0, 38, and 76 within the read. If the source
+material is not barcoded, this field should be marked as "Not applicable".
+Example: 0,38,76</t>
       </text>
     </comment>
     <comment ref="P1" authorId="1">
       <text>
-        <t>(Required) Which read file contains the cell or capture spot barcode. This
-should be included when constructing sequencing libraries with a non-commercial
-kit. This field is required if the source material is barcoded. This field is
-used to determine which analysis pipeline to run.</t>
+        <t>(Required) The sequencing read file contains the cell or capture spot barcode
+sequences. This information is essential when constructing sequencing libraries
+with a non-commercial kit, as it ensures that barcodes are correctly extracted
+during data processing. If the source material is not barcoded, this field
+should be marked as "Not applicable". Example: Read 1 (R1)</t>
       </text>
     </comment>
     <comment ref="Q1" authorId="1">
       <text>
-        <t>(Required) Length of the cell or capture spot barcode in base pairs. Cell and
-capture spot barcodes are, for example, 3 x 8 bp sequences that are spaced by
-constant sequences, the offsets. This should be included when constructing
-sequencing libraries with a non-commercial kit. This field is required if the
-source material is barcoded.  This field is used to determine which analysis
-pipeline to run.</t>
+        <t>(Required) The length of each cell or capture spot barcode in base pairs (bp).
+If the source material is not barcoded, enter "Not applicable". Example: 16</t>
       </text>
     </comment>
     <comment ref="R1" authorId="1">
@@ -193,73 +194,76 @@
     </comment>
     <comment ref="S1" authorId="1">
       <text>
-        <t>(Required) Which read file contains the UMI barcode. This should be included
-when constructing sequencing libraries with a non-commercial kit.</t>
+        <t>(Required) Specifies which sequencing read file contains the Unique Molecular
+Identifier (UMI) barcode. If no UMI is used, enter "Not applicable". Example:
+Read 1 (R1)</t>
       </text>
     </comment>
     <comment ref="T1" authorId="1">
       <text>
-        <t>(Required) Length of the umi barcode in base pairs. This should be included when
-constructing sequencing libraries with a non-commercial kit. This field is
-required if UMI are present. This field is used to determine which analysis
-pipeline to run.</t>
+        <t>(Required) The length of the Unique Molecular Identifier (UMI) in base pairs
+(bp). If no UMI is used, enter "Not applicable". Example: 8</t>
       </text>
     </comment>
     <comment ref="U1" authorId="1">
       <text>
-        <t>(Required) This is the entity from which the analyte is being captured. For
-example, for bulk sequencing this would be "tissue", while it would be "single
-cell" for single cell sequencing. This field is used to determine which analysis
-pipeline to run.</t>
+        <t>(Required) The entity from which the analyte is captured. For example, in bulk
+sequencing, the source entity would be "tissue" while in single-cell sequencing,
+it would be "single cell". Example: single cell</t>
       </text>
     </comment>
     <comment ref="V1" authorId="1">
       <text>
-        <t>How many cells or nuclei were input to the assay? This is typically not
-available for preparations working with bulk tissue.</t>
+        <t>The number of cells or nuclei that were input into the assay. This information
+is typically not available for assays performed on bulk tissue preparations, and
+therefore this field may be left blank. Example: 1000</t>
       </text>
     </comment>
     <comment ref="W1" authorId="1">
       <text>
-        <t>(Required) 5’ and/or 3’ read adapter sequences used as part of the library
-preparation protocol to render the library compatible with the sequencing
-protocol and instrumentation. This should be provided as comma-separated list of
-key:value pairs (adapter name:sequence).</t>
+        <t>(Required) The 5' and/or 3' adapter sequences used during library preparation to
+make the library compatible with the sequencing protocol and instrumentation.
+Adapter sequences should be provided as a comma-separated list of key-value
+pairs in the format: "adapter name: sequence". Example: Nextera Read 1:
+CTGTCTCTTATACACATCT</t>
       </text>
     </comment>
     <comment ref="X1" authorId="1">
       <text>
-        <t>(Required) Average size of sequencing library fragments estimated via gel
-electrophoresis or bioanalyzer/tapestation. Numeric value in base pairs (bp).</t>
+        <t>(Required) The average size of sequencing library fragments, measured in base
+pairs (bp), as estimated by gel electrophoresis, BioAnalyzer, or TapeStation.
+Example: 200</t>
       </text>
     </comment>
     <comment ref="Y1" authorId="1">
       <text>
-        <t>The amount of cDNA, after amplification, that was used for library construction.</t>
+        <t>The amount of cDNA, after amplification, that was used for library construction.
+Example: 60</t>
       </text>
     </comment>
     <comment ref="Z1" authorId="1">
       <text>
-        <t>unit of library input amount value</t>
+        <t>The unit of measurement used to specify the library input amount value. Example:
+ng</t>
       </text>
     </comment>
     <comment ref="AA1" authorId="1">
       <text>
-        <t>Total amount (eg. nanograms) of library after the clean-up step of final pcr
-amplification step. Answer the question: What is the Qubit measured
-concentration (ng/ul) times the elution volume (ul) after the final clean-up
-step?</t>
+        <t>The total amount of library following the clean-up step after the final PCR
+amplification. To calculate, multiply the Qubit-measured concentration (ng/µl)
+by the elution volume (µl) obtained after the final clean-up. Example: 125</t>
       </text>
     </comment>
     <comment ref="AB1" authorId="1">
       <text>
-        <t>Units of library final yield.</t>
+        <t>The unit of measurement used to specify the library output amount value.
+Example: ng</t>
       </text>
     </comment>
     <comment ref="AC1" authorId="1">
       <text>
-        <t>(Required) The concentration value of the pooled library samples submitted for
-sequencing.</t>
+        <t>(Required) The concentration of the pooled library submitted for sequencing.
+Example: 2.5</t>
       </text>
     </comment>
     <comment ref="AD1" authorId="1">
@@ -269,112 +273,131 @@
     </comment>
     <comment ref="AE1" authorId="1">
       <text>
-        <t>(Required) Whether the library was generated for single-end or paired end
-sequencing</t>
+        <t>(Required) Indicates whether the sequencing library was prepared for single-end
+or paired-end sequencing. This information determines how reads are generated
+and aligned during data processing. Example: single-end</t>
       </text>
     </comment>
     <comment ref="AF1" authorId="1">
       <text>
-        <t>(Required) Number of PCR cycles performed in order to add adapters and amplify
-the library. This does not include the cDNA amplification which is captured in
-the "number of iterations of cDNA amplification" field.</t>
+        <t>(Required) The number of PCR cycles used specifically to add sequencing adapters
+and amplify the library during the indexing step. This count does not include
+earlier cDNA amplification cycles, which are recorded separately under the
+"Number of iterations of cDNA amplification" field. Example: 8</t>
       </text>
     </comment>
     <comment ref="AG1" authorId="1">
       <text>
-        <t>(Required) Reagent kit used for library preparation</t>
+        <t>(Required) The reagent kit used to construct the sequencing library, including
+both the kit name and, if available, version and product number. If the library
+was prepared using a custom protocol, enter “Custom”. Example: 10X Genomics;
+Chromium Next GEM Single Cell 5' Kit v2, 16 rxns; PN 1000263</t>
       </text>
     </comment>
     <comment ref="AH1" authorId="1">
       <text>
-        <t>(Required) Indexes are needed for multiplexing sequencing libraries for
-simultaneous sequencing (pooling) and proper attachment to the Illumina
-flowcell. Each indexing kit would have a number of compatible sequences ("sample
-indexing sets") that are used to label some number of samples (the number of
-sets depend on the kit).</t>
+        <t>(Required) The reagent kit used to add index sequences to samples. Indexes
+enable multiplexing, allowing multiple libraries to be pooled and sequenced
+together on the same Illumina flow cell. Each indexing kit includes a set of
+compatible index sequences (often called "indexing sets") used to uniquely label
+a specific number of samples, depending on the kit’s design. If the library was
+prepared using a custom protocol, enter “Custom”. If no indexing was performed,
+enter "Not applicable". Example: 10X Genomics; Dual Index Kit TS, Set A; PN
+1000251</t>
       </text>
     </comment>
     <comment ref="AI1" authorId="1">
       <text>
-        <t>(Required) The specific sequencing barcode index set used, selected from the
-sample indexing kit. Example: For 10X this might be "SI-GA-A1", for Nextera
-"N505 - CTCCTTAC"</t>
+        <t>(Required) The specific sequencing barcode index set used, chosen from the
+sample indexing kit. For example, in the case of 10x, this might be "SI-GA-A1",
+whereas for Nextera, it could be "N505 - CTCCTTAC". Example: SI-GA-A1</t>
       </text>
     </comment>
     <comment ref="AJ1" authorId="1">
       <text>
-        <t>(Required) Is the sequencing reaction run in replicate, "Yes" or "No". If "Yes",
-FASTQ files in dataset need to be merged.</t>
+        <t>(Required) Indicates whether the sequencing reaction was run in replicate. If
+"Yes," the corresponding FASTQ files in the dataset should be merged for
+analysis. Example: Yes</t>
       </text>
     </comment>
     <comment ref="AK1" authorId="1">
       <text>
-        <t>Number of cells, nuclei or capture spots expected to be captured by the assay.
-For Visium this is the total number of spots covered by tissue, within the
-capture area.</t>
+        <t>The number of cells, nuclei, or capture spots expected to be captured by the
+assay. Example: 14336</t>
       </text>
     </comment>
     <comment ref="AL1" authorId="1">
       <text>
-        <t>(Required) Reagent kit used for sequencing</t>
+        <t>(Required) The reagent kit used to perform the sequencing run, including the
+platform, kit name, version, and product number when available. If the reagent
+kit was prepared using a custom protocol, enter “Custom”. Example: Illumina;
+NextSeq 500/550 Hi Output Kit 150 Cycles; v2.5; PN 20024907</t>
       </text>
     </comment>
     <comment ref="AM1" authorId="1">
       <text>
-        <t>(Required) Number of sequencing cycles in each round of sequencing (i.e., Read1,
-i7 index, i5 index, and Read2). This is reported as a comma-delimited list.
-Example: For 10X snATAC-seq (R1,Index,R2,R3) this might be: 50,8,16,50. For
-SNARE-seq2 this might be: 75,94,8,75</t>
+        <t>(Required) The number of sequencing cycles for each read and index in the
+sequencing run, typically reported as a comma-separated list in the order: Read
+1, i7 index, i5 index, and Read 2. Example: 50,8,16,50</t>
       </text>
     </comment>
     <comment ref="AN1" authorId="1">
       <text>
-        <t>(Required) If Tn5 came from a kit, provide the kit details. This should be set
-to "Not applicable" if a custom or in-house kit was used.</t>
+        <t>(Required) The reagent kit used for the transposition step, particularly if Tn5
+transposase was sourced from a commercial kit, including the platform, kit name,
+version, and product number when available. If the reagent kit was prepared
+using a custom protocol, enter “Custom”. if no transposition step, enter "Not
+applicable". Example: 10X Genomics; Chromium NextGem Single Cell Multiome ATAC +
+Gene Expression Reagent Bundle, 16 rxn; PN 1000283</t>
       </text>
     </comment>
     <comment ref="AO1" authorId="1">
       <text>
-        <t>(Required) Modality of capturing accessible chromatin molecules. For example,
-this would be the type of kit that was used.</t>
+        <t>(Required) The method or approach used to capture accessible chromatin regions,
+typically reflecting the type of kit or protocol applied. Example: bulkATACseq</t>
       </text>
     </comment>
     <comment ref="AP1" authorId="1">
       <text>
-        <t>The ID for the sequencing run. This could, for example, be the chip ID and
-should allow users the ability to determine which samples were processed
-together in a sequencing run. It is recommended that data providers prefix the
-ID with the center name, to prevent values overlapping across centers.</t>
+        <t>A lab-assigned identifier for the sequencing run, such as a chip ID, that
+enables users to determine which samples were processed together. To avoid ID
+conflicts across institutions, it is recommended to prefix the ID with the name
+of the sequencing center. Example: Broad_Chip1234</t>
       </text>
     </comment>
     <comment ref="AQ1" authorId="1">
       <text>
-        <t>A lab-generated ID to identify which cells were captured at the same time. This
-would, for example, be an ID to denote which datasets were derived from a single
-10X Genomics Chromium Controller run. In the case of the 10X Controller this
-could be the chip ID and would allow users the ability to determine which
-samples were processed together in a Chromium controller. It is recommended that
-data providers prefix the ID with the center name, to prevent values overlapping
-across centers.</t>
+        <t>A lab-assigned identifier used to indicate which cells or nuclei were captured
+together in the same run. For example, in a 10X Genomics Chromium Controller
+workflow, this could be the chip ID used to trace datasets derived from a single
+capture event. This ID helps users identify samples processed together on the
+same device. To avoid conflicts across institutions, it is recommended to prefix
+the ID with the name of the sequencing center. Example: Broad_Batch1234</t>
       </text>
     </comment>
     <comment ref="AR1" authorId="1">
       <text>
-        <t>The manufacturer of the instrument used to prepare (staining/processing) the
-sample for the assay. If an automatic slide staining method was indicated this
-field should list the manufacturer of the instrument.</t>
+        <t>The company that manufactures the instrument used to prepare the sample (e.g.,
+for staining or other processing steps) prior to the assay. If the instrument
+was custom-built or developed internally, enter "In-House". If no sample
+preparation occurred, enter "Not applicable". Example: 10X Genomics</t>
       </text>
     </comment>
     <comment ref="AS1" authorId="1">
       <text>
-        <t>Manufacturers of a staining system instrument may offer various versions
-(models) of that instrument with different features. Differences in features or
-sensitivities may be relevant to processing or interpretation of the data.</t>
+        <t>The specific model of the instrument used for sample preparation, such as
+staining. Manufacturers may offer multiple models with varying features or
+sensitivities, which can influence how the sample is processed and how the
+resulting data is interpreted. If no sample preparation occurred, enter "Not
+applicable". Example: Chromium X</t>
       </text>
     </comment>
     <comment ref="AT1" authorId="1">
       <text>
-        <t>The reagent kit used with the preparation instrument.</t>
+        <t>The reagent kit used in conjunction with the preparation instrument for sample
+processing (e.g., staining or labeling). If the reagent kit was prepared using a
+custom protocol, enter “Custom”. Example: 10X Genomics; Chromium Next GEM Chip G
+Single Cell Kit, 48 rxns; PN 1000120</t>
       </text>
     </comment>
     <comment ref="AU1" authorId="1">
@@ -389,7 +412,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="659">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="665">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -1516,9 +1539,15 @@
     <t>0,38,76</t>
   </si>
   <si>
+    <t>10,48,78</t>
+  </si>
+  <si>
     <t>10,48,86</t>
   </si>
   <si>
+    <t>0,20-23,41-44</t>
+  </si>
+  <si>
     <t>barcode_read</t>
   </si>
   <si>
@@ -1993,6 +2022,12 @@
     <t>sequencing_reagent_kit</t>
   </si>
   <si>
+    <t>Illumina; NovaSeq X Series 25B Reagent Kit (100 Cycle); PN 20125967</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000463</t>
+  </si>
+  <si>
     <t>Illumina; NovaSeq X Series 1.5B Reagent Kit (300 Cycle); PN 20104705</t>
   </si>
   <si>
@@ -2017,6 +2052,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000352</t>
   </si>
   <si>
+    <t>Illumina; NovaSeq X Series 25B Reagent Kit (200 Cycle); PN 20125968</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000464</t>
+  </si>
+  <si>
     <t>Illumina; NovaSeq X Series 1.5B Reagent Kit (200 Cycle); PN 20104704</t>
   </si>
   <si>
@@ -2359,7 +2400,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-10-17T11:50:25-07:00</t>
+    <t>2025-10-21T12:13:23-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -2582,100 +2623,100 @@
         <v>369</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="AD1" t="s" s="1">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="AE1" t="s" s="1">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="AF1" t="s" s="1">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="AG1" t="s" s="1">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="AH1" t="s" s="1">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="AI1" t="s" s="1">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="AJ1" t="s" s="1">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="AK1" t="s" s="1">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="AL1" t="s" s="1">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="AM1" t="s" s="1">
-        <v>586</v>
+        <v>592</v>
       </c>
       <c r="AN1" t="s" s="1">
-        <v>587</v>
+        <v>593</v>
       </c>
       <c r="AO1" t="s" s="1">
-        <v>588</v>
+        <v>594</v>
       </c>
       <c r="AP1" t="s" s="1">
-        <v>595</v>
+        <v>601</v>
       </c>
       <c r="AQ1" t="s" s="1">
-        <v>596</v>
+        <v>602</v>
       </c>
       <c r="AR1" t="s" s="1">
-        <v>597</v>
+        <v>603</v>
       </c>
       <c r="AS1" t="s" s="1">
-        <v>604</v>
+        <v>610</v>
       </c>
       <c r="AT1" t="s" s="1">
-        <v>631</v>
+        <v>637</v>
       </c>
       <c r="AU1" t="s" s="1">
-        <v>650</v>
+        <v>656</v>
       </c>
     </row>
     <row r="2">
@@ -2683,7 +2724,7 @@
         <v>34</v>
       </c>
       <c r="AU2" t="s" s="48">
-        <v>651</v>
+        <v>657</v>
       </c>
     </row>
   </sheetData>
@@ -2718,7 +2759,7 @@
       <formula1>'time_since_acquisition_instrume'!$A$1:$A$3</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="O2:O1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'barcode_offset'!$A$1:$A$7</formula1>
+      <formula1>'barcode_offset'!$A$1:$A$9</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="P2:P1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'barcode_read'!$A$1:$A$3</formula1>
@@ -2788,7 +2829,7 @@
       <formula2>2147483647</formula2>
     </dataValidation>
     <dataValidation type="list" sqref="AL2:AL1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'sequencing_reagent_kit'!$A$1:$A$27</formula1>
+      <formula1>'sequencing_reagent_kit'!$A$1:$A$29</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AN2:AN1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'transposition_reagent_kit'!$A$1:$A$4</formula1>
@@ -2822,10 +2863,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>378</v>
+        <v>380</v>
       </c>
     </row>
     <row r="2">
@@ -2838,10 +2879,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>380</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -2859,27 +2900,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>382</v>
+        <v>384</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>383</v>
+        <v>385</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>384</v>
+        <v>386</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>385</v>
+        <v>387</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>386</v>
+        <v>388</v>
       </c>
     </row>
     <row r="6">
@@ -2907,12 +2948,12 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>383</v>
+        <v>385</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>388</v>
+        <v>390</v>
       </c>
     </row>
     <row r="4">
@@ -2935,10 +2976,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>378</v>
+        <v>380</v>
       </c>
     </row>
     <row r="2">
@@ -2951,10 +2992,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>380</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -2977,17 +3018,17 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>391</v>
+        <v>393</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>392</v>
+        <v>394</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>393</v>
+        <v>395</v>
       </c>
     </row>
     <row r="5">
@@ -3010,42 +3051,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>396</v>
+        <v>398</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>398</v>
+        <v>400</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>400</v>
+        <v>402</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>402</v>
+        <v>404</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>404</v>
+        <v>406</v>
       </c>
     </row>
   </sheetData>
@@ -3063,18 +3104,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>411</v>
+        <v>413</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>413</v>
+        <v>415</v>
       </c>
     </row>
   </sheetData>
@@ -3092,18 +3133,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>411</v>
+        <v>413</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>413</v>
+        <v>415</v>
       </c>
     </row>
   </sheetData>
@@ -3121,26 +3162,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>419</v>
+        <v>421</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>421</v>
+        <v>423</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>423</v>
+        <v>425</v>
       </c>
     </row>
   </sheetData>
@@ -3158,18 +3199,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>426</v>
+        <v>428</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>428</v>
+        <v>430</v>
       </c>
     </row>
   </sheetData>
@@ -3600,266 +3641,266 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>432</v>
+        <v>434</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>434</v>
+        <v>436</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>436</v>
+        <v>438</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>438</v>
+        <v>440</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>442</v>
+        <v>444</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>444</v>
+        <v>446</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>446</v>
+        <v>448</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>448</v>
+        <v>450</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>450</v>
+        <v>452</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>452</v>
+        <v>454</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>454</v>
+        <v>456</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>456</v>
+        <v>458</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>458</v>
+        <v>460</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>460</v>
+        <v>462</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>462</v>
+        <v>464</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>464</v>
+        <v>466</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>466</v>
+        <v>468</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>468</v>
+        <v>470</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>470</v>
+        <v>472</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>472</v>
+        <v>474</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>474</v>
+        <v>476</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>476</v>
+        <v>478</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>478</v>
+        <v>480</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>480</v>
+        <v>482</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>482</v>
+        <v>484</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>484</v>
+        <v>486</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>486</v>
+        <v>488</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>488</v>
+        <v>490</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>490</v>
+        <v>492</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>492</v>
+        <v>494</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>494</v>
+        <v>496</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>496</v>
+        <v>498</v>
       </c>
     </row>
   </sheetData>
@@ -3877,18 +3918,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>499</v>
+        <v>501</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>501</v>
+        <v>503</v>
       </c>
     </row>
     <row r="3">
@@ -3901,122 +3942,122 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>503</v>
+        <v>505</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>505</v>
+        <v>507</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>507</v>
+        <v>509</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>509</v>
+        <v>511</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>511</v>
+        <v>513</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>513</v>
+        <v>515</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>515</v>
+        <v>517</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>482</v>
+        <v>484</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>517</v>
+        <v>519</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>519</v>
+        <v>521</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>521</v>
+        <v>523</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>523</v>
+        <v>525</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>525</v>
+        <v>527</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>527</v>
+        <v>529</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>529</v>
+        <v>531</v>
       </c>
     </row>
   </sheetData>
@@ -4049,7 +4090,7 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4057,218 +4098,234 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>535</v>
+        <v>537</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>545</v>
+        <v>547</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>547</v>
+        <v>549</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>549</v>
+        <v>551</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>551</v>
+        <v>553</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>553</v>
+        <v>555</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>555</v>
+        <v>557</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>557</v>
+        <v>559</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>559</v>
+        <v>561</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>561</v>
+        <v>563</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>563</v>
+        <v>565</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>481</v>
+        <v>566</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>482</v>
+        <v>567</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>564</v>
+        <v>568</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>565</v>
+        <v>569</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>566</v>
+        <v>483</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>567</v>
+        <v>484</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>569</v>
+        <v>571</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>571</v>
+        <v>573</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>573</v>
+        <v>575</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>575</v>
+        <v>577</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>577</v>
+        <v>579</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>579</v>
+        <v>581</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>581</v>
+        <v>583</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>583</v>
+        <v>585</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>585</v>
+        <v>587</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>588</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>590</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>591</v>
       </c>
     </row>
   </sheetData>
@@ -4286,10 +4343,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>492</v>
+        <v>494</v>
       </c>
     </row>
     <row r="2">
@@ -4302,18 +4359,18 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>478</v>
+        <v>480</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>482</v>
+        <v>484</v>
       </c>
     </row>
   </sheetData>
@@ -4331,34 +4388,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>589</v>
+        <v>595</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>590</v>
+        <v>596</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>591</v>
+        <v>597</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>592</v>
+        <v>598</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>593</v>
+        <v>599</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>594</v>
+        <v>600</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>482</v>
+        <v>484</v>
       </c>
     </row>
   </sheetData>
@@ -4408,18 +4465,18 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>598</v>
+        <v>604</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>599</v>
+        <v>605</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>600</v>
+        <v>606</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>601</v>
+        <v>607</v>
       </c>
     </row>
     <row r="7">
@@ -4440,10 +4497,10 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>602</v>
+        <v>608</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>603</v>
+        <v>609</v>
       </c>
     </row>
   </sheetData>
@@ -4477,10 +4534,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>605</v>
+        <v>611</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>606</v>
+        <v>612</v>
       </c>
     </row>
     <row r="4">
@@ -4493,10 +4550,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>607</v>
+        <v>613</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>608</v>
+        <v>614</v>
       </c>
     </row>
     <row r="6">
@@ -4517,90 +4574,90 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>609</v>
+        <v>615</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>610</v>
+        <v>616</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>611</v>
+        <v>617</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>612</v>
+        <v>618</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>613</v>
+        <v>619</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>614</v>
+        <v>620</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>615</v>
+        <v>621</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>616</v>
+        <v>622</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>618</v>
+        <v>624</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>619</v>
+        <v>625</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>620</v>
+        <v>626</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>621</v>
+        <v>627</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>622</v>
+        <v>628</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>623</v>
+        <v>629</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>624</v>
+        <v>630</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>625</v>
+        <v>631</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>626</v>
+        <v>632</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>627</v>
+        <v>633</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>628</v>
+        <v>634</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>629</v>
+        <v>635</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>630</v>
+        <v>636</v>
       </c>
     </row>
   </sheetData>
@@ -4618,98 +4675,98 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>632</v>
+        <v>638</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>633</v>
+        <v>639</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>634</v>
+        <v>640</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>635</v>
+        <v>641</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>492</v>
+        <v>494</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>636</v>
+        <v>642</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>637</v>
+        <v>643</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>478</v>
+        <v>480</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>638</v>
+        <v>644</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>639</v>
+        <v>645</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>640</v>
+        <v>646</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>641</v>
+        <v>647</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>642</v>
+        <v>648</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>643</v>
+        <v>649</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>644</v>
+        <v>650</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>645</v>
+        <v>651</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>482</v>
+        <v>484</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>646</v>
+        <v>652</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>647</v>
+        <v>653</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>648</v>
+        <v>654</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>649</v>
+        <v>655</v>
       </c>
     </row>
   </sheetData>
@@ -4733,16 +4790,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>652</v>
+        <v>658</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>653</v>
+        <v>659</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>655</v>
+        <v>661</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>657</v>
+        <v>663</v>
       </c>
     </row>
     <row r="2">
@@ -4750,13 +4807,13 @@
         <v>34</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>654</v>
+        <v>660</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>656</v>
+        <v>662</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>658</v>
+        <v>664</v>
       </c>
     </row>
   </sheetData>
@@ -5902,7 +5959,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5940,6 +5997,16 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
         <v>210</v>
       </c>
     </row>

</xml_diff>